<commit_message>
mapping updated with last fixes
</commit_message>
<xml_diff>
--- a/knowledge-graph/mappings/solarchem-mapping.xlsx
+++ b/knowledge-graph/mappings/solarchem-mapping.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aiglesias/GitHub/solarchem-ontology/mappings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aiglesias/GitHub/solarchem-ontology/knowledge-graph/mappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F069437-B2D6-4E48-BBC4-181EFB03A12A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD838C80-644B-C74C-ABD1-6829D44A7608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54160" yWindow="-10300" windowWidth="25840" windowHeight="28300" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-1380" windowWidth="38400" windowHeight="21100" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefix" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,6 @@
   <authors>
     <author>tc={44F07727-749F-3C47-BA2B-19F03CB8B7C7}</author>
     <author>tc={16A91D93-63D0-AF4D-B9FC-79B454B39BC8}</author>
-    <author>tc={695439C3-0C5E-F940-94A3-9E975DD569EF}</author>
   </authors>
   <commentList>
     <comment ref="D12" authorId="0" shapeId="0" xr:uid="{44F07727-749F-3C47-BA2B-19F03CB8B7C7}">
@@ -52,7 +51,7 @@
     Should be float, cannot bc data contains sometimes strings</t>
       </text>
     </comment>
-    <comment ref="B42" authorId="1" shapeId="0" xr:uid="{16A91D93-63D0-AF4D-B9FC-79B454B39BC8}">
+    <comment ref="B41" authorId="1" shapeId="0" xr:uid="{16A91D93-63D0-AF4D-B9FC-79B454B39BC8}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -61,20 +60,12 @@
 </t>
       </text>
     </comment>
-    <comment ref="B73" authorId="2" shapeId="0" xr:uid="{695439C3-0C5E-F940-94A3-9E975DD569EF}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    No encuentro el campo en los datos, igual se calcula on the fly?</t>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="202">
   <si>
     <t>Prefix</t>
   </si>
@@ -427,12 +418,6 @@
     <t>http://w3id.org/solar/i/Input/Dye/{ID}-{Dyes}</t>
   </si>
   <si>
-    <t>solar:depositionMethod</t>
-  </si>
-  <si>
-    <t>{Deposition_method}</t>
-  </si>
-  <si>
     <t>solar:hasBandGap</t>
   </si>
   <si>
@@ -526,9 +511,6 @@
     <t>{ph_value}</t>
   </si>
   <si>
-    <t>solarpc:reactorVolume</t>
-  </si>
-  <si>
     <t>{Reactor_Volume_l}</t>
   </si>
   <si>
@@ -559,9 +541,6 @@
     <t>rdf:type</t>
   </si>
   <si>
-    <t>http://w3id.org/solar/o/pc#{Reactor_type}Reactor</t>
-  </si>
-  <si>
     <t>http://w3id.org/solar/o/core#{Reaction_medium}Medium</t>
   </si>
   <si>
@@ -653,13 +632,52 @@
   </si>
   <si>
     <t>http://w3id.org/solar/i/Input/Reductant/{ID}-{Reductant}</t>
+  </si>
+  <si>
+    <t>{Illuminated_area_m2}</t>
+  </si>
+  <si>
+    <t>ILLUMAREA</t>
+  </si>
+  <si>
+    <t>solar:IlluminatedArea</t>
+  </si>
+  <si>
+    <t>solar:reportedIn</t>
+  </si>
+  <si>
+    <t>http://w3id.org/solar/o/core#{Reactor_type}Reactor</t>
+  </si>
+  <si>
+    <t>http://w3id.org/solar/i/Condition/ReactorVolume/{ID}</t>
+  </si>
+  <si>
+    <t>http://w3id.org/solar/i/Condition/ReactorResidenceTime/{ID}</t>
+  </si>
+  <si>
+    <t>REACTORVOL</t>
+  </si>
+  <si>
+    <t>REACTORRESTIME</t>
+  </si>
+  <si>
+    <t>{Residence_time_min1}</t>
+  </si>
+  <si>
+    <t>unit:PER-MIN</t>
+  </si>
+  <si>
+    <t>solar:ResidenceTimeCondition</t>
+  </si>
+  <si>
+    <t>solar:ReactorVolumeCondition</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -701,12 +719,6 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
@@ -1075,12 +1087,9 @@
   <threadedComment ref="D12" dT="2024-03-22T16:26:13.29" personId="{38DFC2E4-73EA-D74C-967B-80CBA1CEA104}" id="{44F07727-749F-3C47-BA2B-19F03CB8B7C7}">
     <text>Should be float, cannot bc data contains sometimes strings</text>
   </threadedComment>
-  <threadedComment ref="B42" dT="2024-03-23T15:13:35.29" personId="{38DFC2E4-73EA-D74C-967B-80CBA1CEA104}" id="{16A91D93-63D0-AF4D-B9FC-79B454B39BC8}">
+  <threadedComment ref="B41" dT="2024-03-23T15:13:35.29" personId="{38DFC2E4-73EA-D74C-967B-80CBA1CEA104}" id="{16A91D93-63D0-AF4D-B9FC-79B454B39BC8}">
     <text xml:space="preserve">No está en la onto, tiene valor especial con respecto al resto de inputs
 </text>
-  </threadedComment>
-  <threadedComment ref="B73" dT="2024-03-23T15:08:06.85" personId="{38DFC2E4-73EA-D74C-967B-80CBA1CEA104}" id="{695439C3-0C5E-F940-94A3-9E975DD569EF}">
-    <text>No encuentro el campo en los datos, igual se calcula on the fly?</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -1222,10 +1231,10 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1267,10 +1276,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:C25"/>
+    <sheetView topLeftCell="A15" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44:C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1360,7 +1369,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>35</v>
@@ -1371,7 +1380,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>37</v>
@@ -1382,7 +1391,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>35</v>
@@ -1393,7 +1402,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>37</v>
@@ -1536,7 +1545,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>35</v>
@@ -1547,7 +1556,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>37</v>
@@ -1558,7 +1567,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>35</v>
@@ -1569,7 +1578,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>37</v>
@@ -1580,7 +1589,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>35</v>
@@ -1591,7 +1600,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>37</v>
@@ -1602,7 +1611,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>35</v>
@@ -1613,7 +1622,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>37</v>
@@ -1624,7 +1633,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>35</v>
@@ -1635,7 +1644,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>37</v>
@@ -1646,7 +1655,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>35</v>
@@ -1657,7 +1666,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>37</v>
@@ -1668,7 +1677,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>35</v>
@@ -1679,7 +1688,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>37</v>
@@ -1690,7 +1699,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>35</v>
@@ -1701,7 +1710,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>37</v>
@@ -1712,7 +1721,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>35</v>
@@ -1723,12 +1732,78 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>37</v>
       </c>
       <c r="C41" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47" s="7" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1740,16 +1815,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="22.83203125" customWidth="1"/>
+    <col min="2" max="2" width="25.5" customWidth="1"/>
     <col min="3" max="3" width="37.1640625" customWidth="1"/>
     <col min="4" max="1025" width="10.5" customWidth="1"/>
   </cols>
@@ -1801,24 +1876,24 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" t="s">
         <v>123</v>
       </c>
-      <c r="B5" t="s">
-        <v>125</v>
-      </c>
       <c r="C5" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" t="s">
         <v>124</v>
       </c>
-      <c r="B6" t="s">
-        <v>126</v>
-      </c>
       <c r="C6" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1889,105 +1964,141 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B13" t="s">
         <v>67</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B16" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B19" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B20" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B21" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>178</v>
-      </c>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>190</v>
+      </c>
+      <c r="B22" t="s">
+        <v>191</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="B23" t="s">
+        <v>201</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="B24" t="s">
+        <v>200</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="7"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{F1F592FE-66EF-D044-98C4-B07EFAF6846A}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{329341A0-A072-9242-8F6F-A7B5E8616EED}"/>
@@ -2006,10 +2117,12 @@
     <hyperlink ref="C17" r:id="rId15" xr:uid="{2CA5367A-ADF2-3948-A151-F9ED43232B41}"/>
     <hyperlink ref="C18" r:id="rId16" xr:uid="{AF45DD89-DCAB-9D47-82E7-E1514F724422}"/>
     <hyperlink ref="C19" r:id="rId17" xr:uid="{C6281ADE-B007-FF43-987D-BC199502F4A9}"/>
-    <hyperlink ref="C20:C21" r:id="rId18" display="http://w3id.org/solar/i/IlluminatedArea/{ID}" xr:uid="{383A6330-6BEE-9442-B294-451EF5F17054}"/>
-    <hyperlink ref="C20" r:id="rId19" xr:uid="{809DAE46-CFDD-1347-93E9-73C62A907742}"/>
-    <hyperlink ref="C21" r:id="rId20" xr:uid="{A8085152-3BE9-844F-BD28-D23B3F3D0675}"/>
-    <hyperlink ref="C13" r:id="rId21" xr:uid="{CA6E68C4-20B1-9248-AA29-D1A87184FF3B}"/>
+    <hyperlink ref="C20" r:id="rId18" xr:uid="{809DAE46-CFDD-1347-93E9-73C62A907742}"/>
+    <hyperlink ref="C22" r:id="rId19" xr:uid="{A8085152-3BE9-844F-BD28-D23B3F3D0675}"/>
+    <hyperlink ref="C13" r:id="rId20" xr:uid="{CA6E68C4-20B1-9248-AA29-D1A87184FF3B}"/>
+    <hyperlink ref="C21" r:id="rId21" xr:uid="{215F075C-705C-D340-8B34-205253A7FE6F}"/>
+    <hyperlink ref="C24" r:id="rId22" xr:uid="{B26AE112-ECB2-9A41-AAD1-982D7EA177FD}"/>
+    <hyperlink ref="C23" r:id="rId23" xr:uid="{3EC1BB91-66EF-C94B-8ED5-9415761E18F4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2018,10 +2131,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H79"/>
+  <dimension ref="A1:H84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59:C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2272,10 +2385,12 @@
       <c r="B15" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D15" s="7"/>
+      <c r="C15" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
@@ -2285,10 +2400,10 @@
         <v>66</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>119</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>122</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>70</v>
@@ -2299,16 +2414,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>66</v>
+        <v>121</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>121</v>
+        <v>73</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>126</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
@@ -2316,16 +2431,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -2333,16 +2448,16 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -2350,16 +2465,16 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -2367,17 +2482,15 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>124</v>
+        <v>83</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>70</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
@@ -2387,12 +2500,14 @@
         <v>83</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D22" s="7"/>
+        <v>92</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
@@ -2402,13 +2517,13 @@
         <v>83</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
@@ -2416,262 +2531,262 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
+        <v>102</v>
+      </c>
+      <c r="D24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>99</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="D25" s="7"/>
+        <v>92</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>99</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>98</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="D27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>100</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="D28" s="7"/>
+        <v>92</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>100</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>98</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="D30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>85</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D31" s="7"/>
+        <v>87</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>85</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+      <c r="D33" s="7"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>107</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="D34" s="7"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>107</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+      <c r="D36" s="7"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>112</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D37" s="7"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>112</v>
       </c>
       <c r="B38" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D39" s="7"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="B40" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C38" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="D39" s="7" t="s">
+      <c r="C40" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="D41" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="D40" s="7"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>187</v>
+        <v>40</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H42" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
         <v>40</v>
       </c>
@@ -2685,7 +2800,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
         <v>40</v>
       </c>
@@ -2699,7 +2814,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
         <v>40</v>
       </c>
@@ -2713,7 +2828,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
         <v>40</v>
       </c>
@@ -2727,7 +2842,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>40</v>
       </c>
@@ -2741,7 +2856,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
         <v>40</v>
       </c>
@@ -2777,7 +2892,7 @@
         <v>64</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>70</v>
@@ -2788,10 +2903,10 @@
         <v>40</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>70</v>
@@ -2802,10 +2917,10 @@
         <v>40</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>70</v>
@@ -2816,10 +2931,10 @@
         <v>40</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>135</v>
+        <v>193</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>70</v>
@@ -2830,10 +2945,10 @@
         <v>40</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>70</v>
@@ -2844,10 +2959,10 @@
         <v>40</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D55" s="7" t="s">
         <v>70</v>
@@ -2858,10 +2973,10 @@
         <v>40</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D56" s="7" t="s">
         <v>70</v>
@@ -2872,10 +2987,10 @@
         <v>40</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D57" s="7" t="s">
         <v>70</v>
@@ -2886,10 +3001,10 @@
         <v>40</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D58" s="7" t="s">
         <v>70</v>
@@ -2897,27 +3012,27 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
-        <v>139</v>
+        <v>40</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C59" s="7" t="s">
-        <v>149</v>
+        <v>129</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>194</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
-        <v>139</v>
+        <v>40</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>159</v>
+        <v>129</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>195</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>70</v>
@@ -2925,13 +3040,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>150</v>
+        <v>73</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D61" s="7" t="s">
         <v>98</v>
@@ -2939,13 +3054,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>75</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D62" s="7" t="s">
         <v>70</v>
@@ -2953,111 +3068,111 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
-        <v>140</v>
+        <v>196</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>161</v>
+        <v>73</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>148</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
-        <v>141</v>
+        <v>196</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
-        <v>141</v>
+        <v>197</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>156</v>
+        <v>198</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
-        <v>142</v>
+        <v>197</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>153</v>
+        <v>199</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="7" t="s">
-        <v>164</v>
+        <v>140</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="C70" s="8" t="s">
-        <v>168</v>
+        <v>75</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>154</v>
       </c>
       <c r="D70" s="7" t="s">
         <v>70</v>
@@ -3065,27 +3180,27 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="s">
-        <v>164</v>
+        <v>141</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="C71" s="8" t="s">
-        <v>170</v>
+        <v>73</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>151</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
-        <v>164</v>
+        <v>141</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="C72" s="8" t="s">
-        <v>175</v>
+        <v>75</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>152</v>
       </c>
       <c r="D72" s="7" t="s">
         <v>70</v>
@@ -3093,13 +3208,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C73" s="8" t="s">
         <v>164</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="C73" s="8" t="s">
-        <v>176</v>
       </c>
       <c r="D73" s="7" t="s">
         <v>70</v>
@@ -3107,13 +3222,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="7" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="D74" s="7" t="s">
         <v>70</v>
@@ -3121,13 +3236,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="D75" s="7" t="s">
         <v>70</v>
@@ -3135,27 +3250,27 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C76" s="7" t="s">
-        <v>183</v>
+        <v>170</v>
+      </c>
+      <c r="C76" s="8" t="s">
+        <v>172</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C77" s="7" t="s">
-        <v>185</v>
+        <v>169</v>
+      </c>
+      <c r="C77" s="8" t="s">
+        <v>173</v>
       </c>
       <c r="D77" s="7" t="s">
         <v>70</v>
@@ -3163,34 +3278,104 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="7" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C78" s="7" t="s">
-        <v>184</v>
+        <v>168</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>174</v>
       </c>
       <c r="D78" s="7" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D79" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="D80" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C81" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="B79" s="7" t="s">
+      <c r="D81" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B82" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C79" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="D79" s="7" t="s">
+      <c r="C82" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="D82" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="D83" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="D84" s="7" t="s">
         <v>70</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C43" r:id="rId1" xr:uid="{33CD0375-FDC4-864D-8BAE-CF58136577F6}"/>
     <hyperlink ref="C44" r:id="rId2" xr:uid="{87955B5B-4B6D-4B4A-B115-3F447052E311}"/>
@@ -3199,29 +3384,30 @@
     <hyperlink ref="C46" r:id="rId5" xr:uid="{26286F07-CF01-3D4F-AF7E-24B1DFF4CAC5}"/>
     <hyperlink ref="C48" r:id="rId6" xr:uid="{250FC759-8E91-AD4E-BB93-AAF3872DC404}"/>
     <hyperlink ref="C50" r:id="rId7" xr:uid="{5D2E891D-0452-324E-AC63-3B5EB8FCC576}"/>
-    <hyperlink ref="C16" r:id="rId8" xr:uid="{B83A9430-8469-3340-8A32-6DDD9D53D7BD}"/>
-    <hyperlink ref="C17" r:id="rId9" xr:uid="{699A6F69-F379-0348-B5C9-C25D7DB140FB}"/>
+    <hyperlink ref="C15" r:id="rId8" xr:uid="{B83A9430-8469-3340-8A32-6DDD9D53D7BD}"/>
+    <hyperlink ref="C16" r:id="rId9" xr:uid="{699A6F69-F379-0348-B5C9-C25D7DB140FB}"/>
     <hyperlink ref="C51" r:id="rId10" xr:uid="{EFCC2B08-8773-C547-9417-6D50A357579D}"/>
     <hyperlink ref="C52" r:id="rId11" xr:uid="{4ED7AA7D-0161-9048-913F-4E262F489078}"/>
-    <hyperlink ref="C53" r:id="rId12" xr:uid="{055C092E-EA3C-784C-9752-B62AF65DB27F}"/>
-    <hyperlink ref="C54" r:id="rId13" xr:uid="{D4B94815-2A3D-554A-9A3A-D6C41768932F}"/>
-    <hyperlink ref="C55" r:id="rId14" xr:uid="{B9A4BC97-C4E7-CB40-BDEE-3FC54B1A15F8}"/>
-    <hyperlink ref="C56" r:id="rId15" xr:uid="{1A254817-AA29-4349-9F3D-1F08E4B7BC6D}"/>
-    <hyperlink ref="C63" r:id="rId16" location="{Reactor_type}Reactor" xr:uid="{0AB9E7B4-D674-2E47-9B72-341D1022B491}"/>
-    <hyperlink ref="C57" r:id="rId17" location="{Reaction_medium}Medium" xr:uid="{9FFFB41F-40DA-E844-8105-33FA71783875}"/>
-    <hyperlink ref="C58" r:id="rId18" location="{Operation_mode}Mode" xr:uid="{E49C1ABB-2410-D945-BAD5-E813751ECA22}"/>
-    <hyperlink ref="C70" r:id="rId19" location="{Light_source}LightSource" xr:uid="{5D5BAA03-A593-D246-AA1D-DD5A58EEB0FF}"/>
-    <hyperlink ref="C71" r:id="rId20" location="{Lamp}Lamp" xr:uid="{B474DE65-6CF2-6449-8CB9-C1A8F1227029}"/>
-    <hyperlink ref="C72" r:id="rId21" location="{Wavelength_nm}WL" xr:uid="{CDAAFAD0-E55A-C64F-A0E5-874107AAA07C}"/>
-    <hyperlink ref="C73" r:id="rId22" xr:uid="{D635B011-750E-414E-91E7-5327241CF37A}"/>
-    <hyperlink ref="C74:C75" r:id="rId23" display="http://w3id.org/solar/i/IlluminatedArea/{ID}" xr:uid="{4DFEDC35-DAA6-804C-B0F6-2CAF9BC91727}"/>
-    <hyperlink ref="C74" r:id="rId24" xr:uid="{1D48B95E-8BAD-E044-A7A5-74EFE823C221}"/>
-    <hyperlink ref="C75" r:id="rId25" xr:uid="{6118BC49-CEA9-7C4E-ABE8-63EA5ED604C9}"/>
-    <hyperlink ref="C49" r:id="rId26" xr:uid="{BD436ABE-9765-184F-AB49-2AAD056EA2AC}"/>
+    <hyperlink ref="C54" r:id="rId12" xr:uid="{D4B94815-2A3D-554A-9A3A-D6C41768932F}"/>
+    <hyperlink ref="C55" r:id="rId13" xr:uid="{B9A4BC97-C4E7-CB40-BDEE-3FC54B1A15F8}"/>
+    <hyperlink ref="C56" r:id="rId14" xr:uid="{1A254817-AA29-4349-9F3D-1F08E4B7BC6D}"/>
+    <hyperlink ref="C57" r:id="rId15" location="{Reaction_medium}Medium" xr:uid="{9FFFB41F-40DA-E844-8105-33FA71783875}"/>
+    <hyperlink ref="C58" r:id="rId16" location="{Operation_mode}Mode" xr:uid="{E49C1ABB-2410-D945-BAD5-E813751ECA22}"/>
+    <hyperlink ref="C73" r:id="rId17" location="{Light_source}LightSource" xr:uid="{5D5BAA03-A593-D246-AA1D-DD5A58EEB0FF}"/>
+    <hyperlink ref="C74" r:id="rId18" location="{Lamp}Lamp" xr:uid="{B474DE65-6CF2-6449-8CB9-C1A8F1227029}"/>
+    <hyperlink ref="C75" r:id="rId19" location="{Wavelength_nm}WL" xr:uid="{CDAAFAD0-E55A-C64F-A0E5-874107AAA07C}"/>
+    <hyperlink ref="C76" r:id="rId20" xr:uid="{D635B011-750E-414E-91E7-5327241CF37A}"/>
+    <hyperlink ref="C77:C78" r:id="rId21" display="http://w3id.org/solar/i/IlluminatedArea/{ID}" xr:uid="{4DFEDC35-DAA6-804C-B0F6-2CAF9BC91727}"/>
+    <hyperlink ref="C77" r:id="rId22" xr:uid="{1D48B95E-8BAD-E044-A7A5-74EFE823C221}"/>
+    <hyperlink ref="C78" r:id="rId23" xr:uid="{6118BC49-CEA9-7C4E-ABE8-63EA5ED604C9}"/>
+    <hyperlink ref="C49" r:id="rId24" xr:uid="{BD436ABE-9765-184F-AB49-2AAD056EA2AC}"/>
+    <hyperlink ref="C53" r:id="rId25" location="{Reactor_type}Reactor" xr:uid="{12796564-401A-904D-BA88-6DE0252945FE}"/>
+    <hyperlink ref="C60" r:id="rId26" xr:uid="{4A57F8C9-3F6B-F346-9C06-14ACCD76C291}"/>
+    <hyperlink ref="C59" r:id="rId27" xr:uid="{D05AEF8F-000B-5243-AA02-25149BFE83E8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <legacyDrawing r:id="rId27"/>
+  <legacyDrawing r:id="rId28"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
catalyst mass datatype fixed
</commit_message>
<xml_diff>
--- a/knowledge-graph/mappings/solarchem-mapping.xlsx
+++ b/knowledge-graph/mappings/solarchem-mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aiglesias/GitHub/solarchem-ontology/knowledge-graph/mappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD838C80-644B-C74C-ABD1-6829D44A7608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD218726-25D4-A04B-91EA-BABA7864D7BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-1380" windowWidth="38400" windowHeight="21100" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,19 +39,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={44F07727-749F-3C47-BA2B-19F03CB8B7C7}</author>
     <author>tc={16A91D93-63D0-AF4D-B9FC-79B454B39BC8}</author>
   </authors>
   <commentList>
-    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{44F07727-749F-3C47-BA2B-19F03CB8B7C7}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Should be float, cannot bc data contains sometimes strings</t>
-      </text>
-    </comment>
-    <comment ref="B41" authorId="1" shapeId="0" xr:uid="{16A91D93-63D0-AF4D-B9FC-79B454B39BC8}">
+    <comment ref="B41" authorId="0" shapeId="0" xr:uid="{16A91D93-63D0-AF4D-B9FC-79B454B39BC8}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -65,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="202">
   <si>
     <t>Prefix</t>
   </si>
@@ -1084,9 +1075,6 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D12" dT="2024-03-22T16:26:13.29" personId="{38DFC2E4-73EA-D74C-967B-80CBA1CEA104}" id="{44F07727-749F-3C47-BA2B-19F03CB8B7C7}">
-    <text>Should be float, cannot bc data contains sometimes strings</text>
-  </threadedComment>
   <threadedComment ref="B41" dT="2024-03-23T15:13:35.29" personId="{38DFC2E4-73EA-D74C-967B-80CBA1CEA104}" id="{16A91D93-63D0-AF4D-B9FC-79B454B39BC8}">
     <text xml:space="preserve">No está en la onto, tiene valor especial con respecto al resto de inputs
 </text>
@@ -2133,8 +2121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59:C60"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2341,7 +2329,9 @@
       <c r="C12" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D12" s="7"/>
+      <c r="D12" s="7" t="s">
+        <v>98</v>
+      </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>

</xml_diff>

<commit_message>
minor fixes in mappings and notebook
</commit_message>
<xml_diff>
--- a/knowledge-graph/mappings/solarchem-mapping.xlsx
+++ b/knowledge-graph/mappings/solarchem-mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aiglesias/GitHub/solarchem-ontology/knowledge-graph/mappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD218726-25D4-A04B-91EA-BABA7864D7BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45137A3-AF09-4C4F-9668-239327E8751C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-1380" windowWidth="38400" windowHeight="21100" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-1020" windowWidth="38400" windowHeight="21100" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefix" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="203">
   <si>
     <t>Prefix</t>
   </si>
@@ -289,9 +289,6 @@
     <t>qudt</t>
   </si>
   <si>
-    <t>http://qudt.org/2.1/schema/qudt</t>
-  </si>
-  <si>
     <t>unit</t>
   </si>
   <si>
@@ -662,6 +659,12 @@
   </si>
   <si>
     <t>solar:ReactorVolumeCondition</t>
+  </si>
+  <si>
+    <t>http://qudt.org/2.1/schema/qudt/</t>
+  </si>
+  <si>
+    <t>unit:M2</t>
   </si>
 </sst>
 </file>
@@ -1087,7 +1090,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1179,7 +1182,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>33</v>
@@ -1206,23 +1209,23 @@
         <v>76</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>77</v>
+        <v>201</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1357,7 +1360,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>35</v>
@@ -1368,7 +1371,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>37</v>
@@ -1379,7 +1382,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>35</v>
@@ -1390,7 +1393,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>37</v>
@@ -1401,7 +1404,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>35</v>
@@ -1412,7 +1415,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>37</v>
@@ -1423,7 +1426,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>35</v>
@@ -1434,7 +1437,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>37</v>
@@ -1445,7 +1448,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>35</v>
@@ -1456,7 +1459,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>37</v>
@@ -1467,7 +1470,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>35</v>
@@ -1478,7 +1481,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>37</v>
@@ -1489,7 +1492,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>35</v>
@@ -1500,7 +1503,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>37</v>
@@ -1511,7 +1514,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>35</v>
@@ -1522,7 +1525,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>37</v>
@@ -1533,7 +1536,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>35</v>
@@ -1544,7 +1547,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>37</v>
@@ -1555,7 +1558,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>35</v>
@@ -1566,7 +1569,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>37</v>
@@ -1577,7 +1580,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>35</v>
@@ -1588,7 +1591,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>37</v>
@@ -1599,7 +1602,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>35</v>
@@ -1610,7 +1613,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>37</v>
@@ -1621,7 +1624,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>35</v>
@@ -1632,7 +1635,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>37</v>
@@ -1643,7 +1646,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>35</v>
@@ -1654,7 +1657,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>37</v>
@@ -1665,7 +1668,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>35</v>
@@ -1676,7 +1679,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>37</v>
@@ -1687,7 +1690,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>35</v>
@@ -1698,7 +1701,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>37</v>
@@ -1709,7 +1712,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>35</v>
@@ -1720,7 +1723,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>37</v>
@@ -1731,7 +1734,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>35</v>
@@ -1742,7 +1745,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>37</v>
@@ -1753,7 +1756,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>35</v>
@@ -1764,7 +1767,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>37</v>
@@ -1775,7 +1778,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>35</v>
@@ -1786,7 +1789,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>37</v>
@@ -1859,227 +1862,227 @@
         <v>67</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
         <v>67</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B8" t="s">
         <v>67</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
         <v>67</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B10" t="s">
         <v>67</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B11" t="s">
         <v>67</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B12" t="s">
         <v>67</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B13" t="s">
         <v>67</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B20" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B21" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>189</v>
+      </c>
+      <c r="B22" t="s">
         <v>190</v>
       </c>
-      <c r="B22" t="s">
-        <v>191</v>
-      </c>
       <c r="C22" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -2121,8 +2124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2277,7 +2280,9 @@
         <v>58</v>
       </c>
       <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+      <c r="D9" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="F9" s="7" t="s">
         <v>40</v>
       </c>
@@ -2293,10 +2298,10 @@
         <v>66</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>80</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -2330,7 +2335,7 @@
         <v>74</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -2344,7 +2349,7 @@
         <v>75</v>
       </c>
       <c r="C13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>70</v>
@@ -2358,10 +2363,10 @@
         <v>66</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -2373,10 +2378,10 @@
         <v>66</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>70</v>
@@ -2390,10 +2395,10 @@
         <v>66</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>118</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>119</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>70</v>
@@ -2404,16 +2409,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>73</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
@@ -2421,13 +2426,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>75</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>70</v>
@@ -2438,16 +2443,16 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>73</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -2455,13 +2460,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>75</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>70</v>
@@ -2472,13 +2477,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
@@ -2487,13 +2492,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>68</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>70</v>
@@ -2504,16 +2509,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>84</v>
-      </c>
       <c r="C23" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
@@ -2521,25 +2526,25 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>68</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>70</v>
@@ -2547,39 +2552,39 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>68</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>70</v>
@@ -2587,39 +2592,39 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="7" t="s">
         <v>85</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>86</v>
       </c>
       <c r="D30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>68</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>70</v>
@@ -2627,39 +2632,39 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D33" s="7"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>68</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>70</v>
@@ -2667,39 +2672,39 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D36" s="7"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>68</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>70</v>
@@ -2707,39 +2712,39 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" s="7" t="s">
         <v>183</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>184</v>
       </c>
       <c r="D39" s="7"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>68</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>70</v>
@@ -2747,16 +2752,16 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B41" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="C41" s="7" t="s">
-        <v>187</v>
-      </c>
       <c r="D41" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -2764,7 +2769,10 @@
         <v>40</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="F42" s="9" t="s">
         <v>34</v>
@@ -2784,7 +2792,7 @@
         <v>64</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>70</v>
@@ -2798,7 +2806,7 @@
         <v>64</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>70</v>
@@ -2812,7 +2820,7 @@
         <v>64</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>70</v>
@@ -2826,7 +2834,7 @@
         <v>64</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>70</v>
@@ -2840,7 +2848,7 @@
         <v>64</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>70</v>
@@ -2854,7 +2862,7 @@
         <v>64</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>70</v>
@@ -2868,7 +2876,7 @@
         <v>64</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>70</v>
@@ -2882,7 +2890,7 @@
         <v>64</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>70</v>
@@ -2893,10 +2901,10 @@
         <v>40</v>
       </c>
       <c r="B51" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C51" s="8" t="s">
         <v>131</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>132</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>70</v>
@@ -2907,10 +2915,10 @@
         <v>40</v>
       </c>
       <c r="B52" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C52" s="8" t="s">
         <v>129</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>130</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>70</v>
@@ -2921,10 +2929,10 @@
         <v>40</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>70</v>
@@ -2935,10 +2943,10 @@
         <v>40</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>70</v>
@@ -2949,10 +2957,10 @@
         <v>40</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D55" s="7" t="s">
         <v>70</v>
@@ -2963,10 +2971,10 @@
         <v>40</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D56" s="7" t="s">
         <v>70</v>
@@ -2977,10 +2985,10 @@
         <v>40</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D57" s="7" t="s">
         <v>70</v>
@@ -2991,10 +2999,10 @@
         <v>40</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D58" s="7" t="s">
         <v>70</v>
@@ -3005,10 +3013,10 @@
         <v>40</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D59" s="7" t="s">
         <v>70</v>
@@ -3019,10 +3027,10 @@
         <v>40</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>70</v>
@@ -3030,27 +3038,27 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>73</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>75</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D62" s="7" t="s">
         <v>70</v>
@@ -3058,27 +3066,27 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B63" s="7" t="s">
         <v>73</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B64" s="7" t="s">
         <v>75</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D64" s="7" t="s">
         <v>70</v>
@@ -3086,27 +3094,27 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B65" s="7" t="s">
         <v>73</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B66" s="7" t="s">
         <v>75</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D66" s="7" t="s">
         <v>70</v>
@@ -3114,27 +3122,27 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>73</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B68" s="7" t="s">
         <v>75</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D68" s="7" t="s">
         <v>70</v>
@@ -3142,27 +3150,27 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B69" s="7" t="s">
         <v>73</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B70" s="7" t="s">
         <v>75</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D70" s="7" t="s">
         <v>70</v>
@@ -3170,27 +3178,27 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B71" s="7" t="s">
         <v>73</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B72" s="7" t="s">
         <v>75</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D72" s="7" t="s">
         <v>70</v>
@@ -3198,13 +3206,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D73" s="7" t="s">
         <v>70</v>
@@ -3212,13 +3220,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B74" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C74" s="8" t="s">
         <v>165</v>
-      </c>
-      <c r="C74" s="8" t="s">
-        <v>166</v>
       </c>
       <c r="D74" s="7" t="s">
         <v>70</v>
@@ -3226,13 +3234,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D75" s="7" t="s">
         <v>70</v>
@@ -3240,13 +3248,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D76" s="7" t="s">
         <v>70</v>
@@ -3254,13 +3262,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D77" s="7" t="s">
         <v>70</v>
@@ -3268,13 +3276,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D78" s="7" t="s">
         <v>70</v>
@@ -3282,27 +3290,27 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B79" s="7" t="s">
         <v>73</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B80" s="7" t="s">
         <v>75</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D80" s="7" t="s">
         <v>70</v>
@@ -3310,27 +3318,27 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B81" s="7" t="s">
         <v>73</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B82" s="7" t="s">
         <v>75</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D82" s="7" t="s">
         <v>70</v>
@@ -3338,27 +3346,27 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B83" s="7" t="s">
         <v>73</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D83" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B84" s="7" t="s">
         <v>75</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>182</v>
+        <v>202</v>
       </c>
       <c r="D84" s="7" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
mappings updated with SOA
</commit_message>
<xml_diff>
--- a/knowledge-graph/mappings/solarchem-mapping.xlsx
+++ b/knowledge-graph/mappings/solarchem-mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aiglesias/GitHub/solarchem-ontology/knowledge-graph/mappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45137A3-AF09-4C4F-9668-239327E8751C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFC1055-417C-3D45-A69E-D5C00C4EADBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-1020" windowWidth="38400" windowHeight="21100" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38420" yWindow="-1020" windowWidth="38400" windowHeight="21100" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefix" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
     <author>tc={16A91D93-63D0-AF4D-B9FC-79B454B39BC8}</author>
   </authors>
   <commentList>
-    <comment ref="B41" authorId="0" shapeId="0" xr:uid="{16A91D93-63D0-AF4D-B9FC-79B454B39BC8}">
+    <comment ref="B34" authorId="0" shapeId="0" xr:uid="{16A91D93-63D0-AF4D-B9FC-79B454B39BC8}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="188">
   <si>
     <t>Prefix</t>
   </si>
@@ -166,9 +166,6 @@
     <t>source</t>
   </si>
   <si>
-    <t>data/paper_references.csv</t>
-  </si>
-  <si>
     <t>format</t>
   </si>
   <si>
@@ -190,60 +187,12 @@
     <t>bibo:Article</t>
   </si>
   <si>
-    <t>bibo:doi</t>
-  </si>
-  <si>
-    <t>bibo:abstract</t>
-  </si>
-  <si>
-    <t>bibo:volume</t>
-  </si>
-  <si>
-    <t>dc:title</t>
-  </si>
-  <si>
-    <t>bibo:issue</t>
-  </si>
-  <si>
-    <t>dc:date</t>
-  </si>
-  <si>
-    <t>bibo:pageStart</t>
-  </si>
-  <si>
-    <t>{DOI}</t>
-  </si>
-  <si>
-    <t>{Title}</t>
-  </si>
-  <si>
-    <t>gYear</t>
-  </si>
-  <si>
-    <t>{Pages}</t>
-  </si>
-  <si>
-    <t>{Year}</t>
-  </si>
-  <si>
-    <t>{Issue}</t>
-  </si>
-  <si>
-    <t>{Volume}</t>
-  </si>
-  <si>
     <t>solar:hasExperimentExecution</t>
   </si>
   <si>
     <t>Language</t>
   </si>
   <si>
-    <t>{Abstract}</t>
-  </si>
-  <si>
-    <t>http://w3id.org/solar/i/Article/{No_de_Ref}</t>
-  </si>
-  <si>
     <t>solar:ExperimentExecution</t>
   </si>
   <si>
@@ -665,6 +614,12 @@
   </si>
   <si>
     <t>unit:M2</t>
+  </si>
+  <si>
+    <t>{SOA_URI}</t>
+  </si>
+  <si>
+    <t>data/paper_references_soa.csv</t>
   </si>
 </sst>
 </file>
@@ -1078,7 +1033,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="B41" dT="2024-03-23T15:13:35.29" personId="{38DFC2E4-73EA-D74C-967B-80CBA1CEA104}" id="{16A91D93-63D0-AF4D-B9FC-79B454B39BC8}">
+  <threadedComment ref="B34" dT="2024-03-23T15:13:35.29" personId="{38DFC2E4-73EA-D74C-967B-80CBA1CEA104}" id="{16A91D93-63D0-AF4D-B9FC-79B454B39BC8}">
     <text xml:space="preserve">No está en la onto, tiene valor especial con respecto al resto de inputs
 </text>
   </threadedComment>
@@ -1182,7 +1137,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>33</v>
@@ -1190,42 +1145,42 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>201</v>
+        <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1269,8 +1224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44:C47"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1300,7 +1255,7 @@
         <v>35</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>36</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1308,494 +1263,494 @@
         <v>34</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1809,7 +1764,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1837,252 +1792,252 @@
         <v>34</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>61</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="B5" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="B6" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="B14" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="B15" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="B16" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="B17" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="B18" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="B19" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="B20" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="B21" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="B22" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="B23" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
       <c r="B24" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -2091,7 +2046,7 @@
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{F1F592FE-66EF-D044-98C4-B07EFAF6846A}"/>
+    <hyperlink ref="C2" r:id="rId1" display="http://w3id.org/solar/i/Article/{SOA_URI}" xr:uid="{F1F592FE-66EF-D044-98C4-B07EFAF6846A}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{329341A0-A072-9242-8F6F-A7B5E8616EED}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{02AE9908-CF19-CB41-8387-762706A65FB6}"/>
     <hyperlink ref="C7" r:id="rId4" xr:uid="{4B69325E-4848-5C4A-97E8-083D91448168}"/>
@@ -2122,10 +2077,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H84"/>
+  <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2153,7 +2108,7 @@
         <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>14</v>
@@ -2170,138 +2125,148 @@
         <v>34</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
+        <v>43</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
-        <v>34</v>
+      <c r="A3" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" s="7"/>
+        <v>62</v>
+      </c>
+      <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
-        <v>34</v>
+      <c r="A4" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" s="7"/>
+        <v>52</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
-        <v>34</v>
+      <c r="A5" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="7"/>
+        <v>57</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
-        <v>34</v>
+      <c r="A6" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" s="7"/>
+        <v>58</v>
+      </c>
+      <c r="C6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
-        <v>34</v>
+      <c r="A7" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>53</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
-        <v>34</v>
+      <c r="A8" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="7"/>
+        <v>99</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
-        <v>34</v>
+      <c r="A9" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" s="7"/>
+        <v>100</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>101</v>
+      </c>
       <c r="D9" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>63</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>79</v>
+        <v>108</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -2309,16 +2274,16 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>69</v>
+        <v>109</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -2326,16 +2291,16 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>66</v>
+        <v>104</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>74</v>
+        <v>107</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -2343,16 +2308,16 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>66</v>
+        <v>104</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C13" t="s">
-        <v>88</v>
+        <v>58</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>110</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -2360,13 +2325,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -2375,16 +2340,16 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>119</v>
+        <v>51</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
@@ -2392,1016 +2357,899 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>118</v>
+      <c r="C16" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>120</v>
+        <v>81</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>120</v>
+        <v>81</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>126</v>
+        <v>74</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>121</v>
+        <v>81</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>124</v>
+        <v>83</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>121</v>
+        <v>82</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>82</v>
       </c>
       <c r="B22" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="D23" s="7"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C23" s="7" t="s">
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D27" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="D24" s="7"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="D27" s="7"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D29" s="7"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D30" s="7"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>84</v>
+        <v>165</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>97</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="D32" s="7"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>106</v>
+        <v>165</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="D33" s="7"/>
+        <v>167</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>106</v>
+        <v>165</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>68</v>
+        <v>168</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>109</v>
+        <v>169</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>106</v>
+        <v>39</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>110</v>
+        <v>174</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>97</v>
+        <v>53</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>111</v>
+        <v>39</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="D36" s="7"/>
+        <v>47</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>111</v>
+        <v>39</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>112</v>
+        <v>47</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>111</v>
+        <v>39</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>113</v>
+        <v>47</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>97</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
-        <v>182</v>
+        <v>39</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="D39" s="7"/>
+        <v>47</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>182</v>
+        <v>39</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>184</v>
+        <v>47</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>182</v>
+        <v>39</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>186</v>
+        <v>47</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>97</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>191</v>
+        <v>47</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G42" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="H42" s="7" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>94</v>
+        <v>170</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>64</v>
+        <v>113</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>64</v>
+        <v>111</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>64</v>
+        <v>111</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>105</v>
+        <v>175</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>64</v>
+        <v>111</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>64</v>
+        <v>111</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>64</v>
+        <v>111</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>64</v>
+        <v>111</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>187</v>
+        <v>140</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>129</v>
+        <v>176</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
-        <v>40</v>
+        <v>119</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>133</v>
+        <v>56</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>129</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
-        <v>40</v>
+        <v>119</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>134</v>
+        <v>58</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
-        <v>40</v>
+        <v>178</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>135</v>
+        <v>56</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>130</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
-        <v>40</v>
+        <v>178</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>157</v>
+        <v>58</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
-        <v>40</v>
+        <v>179</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>158</v>
+        <v>56</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>180</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
-        <v>40</v>
+        <v>179</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>193</v>
+        <v>58</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>181</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
-        <v>40</v>
+        <v>121</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>194</v>
+        <v>56</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>97</v>
+        <v>53</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>155</v>
+        <v>132</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
-        <v>195</v>
+        <v>122</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>97</v>
+        <v>53</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
-        <v>195</v>
+        <v>123</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
-        <v>196</v>
+        <v>123</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>197</v>
+        <v>134</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>97</v>
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
-        <v>196</v>
+        <v>142</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>198</v>
+        <v>139</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>146</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C67" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C67" s="8" t="s">
         <v>148</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>97</v>
+        <v>53</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>153</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C69" s="7" t="s">
-        <v>149</v>
+        <v>152</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>154</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>97</v>
+        <v>53</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="7" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C70" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>155</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C71" s="7" t="s">
         <v>150</v>
       </c>
+      <c r="C71" s="8" t="s">
+        <v>156</v>
+      </c>
       <c r="D71" s="7" t="s">
-        <v>97</v>
+        <v>53</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
-        <v>140</v>
+        <v>157</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="C73" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C73" s="7" t="s">
         <v>163</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="C74" s="8" t="s">
-        <v>165</v>
+        <v>56</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>162</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="C75" s="8" t="s">
-        <v>170</v>
+        <v>58</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>164</v>
       </c>
       <c r="D75" s="7" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="C76" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C76" s="7" t="s">
         <v>171</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="C77" s="8" t="s">
-        <v>172</v>
+        <v>58</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>185</v>
       </c>
       <c r="D77" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="C78" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="D78" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="D79" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="D80" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="D81" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="B82" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="D82" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="B83" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C83" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="D83" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="B84" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C84" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="D84" s="7" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C43" r:id="rId1" xr:uid="{33CD0375-FDC4-864D-8BAE-CF58136577F6}"/>
-    <hyperlink ref="C44" r:id="rId2" xr:uid="{87955B5B-4B6D-4B4A-B115-3F447052E311}"/>
-    <hyperlink ref="C47" r:id="rId3" xr:uid="{3D40A9A3-79A8-4048-A619-0101D21BBBDB}"/>
-    <hyperlink ref="C45" r:id="rId4" xr:uid="{DF6AE900-F5E5-1A46-90FE-9B17C12CD5EA}"/>
-    <hyperlink ref="C46" r:id="rId5" xr:uid="{26286F07-CF01-3D4F-AF7E-24B1DFF4CAC5}"/>
-    <hyperlink ref="C48" r:id="rId6" xr:uid="{250FC759-8E91-AD4E-BB93-AAF3872DC404}"/>
-    <hyperlink ref="C50" r:id="rId7" xr:uid="{5D2E891D-0452-324E-AC63-3B5EB8FCC576}"/>
-    <hyperlink ref="C15" r:id="rId8" xr:uid="{B83A9430-8469-3340-8A32-6DDD9D53D7BD}"/>
-    <hyperlink ref="C16" r:id="rId9" xr:uid="{699A6F69-F379-0348-B5C9-C25D7DB140FB}"/>
-    <hyperlink ref="C51" r:id="rId10" xr:uid="{EFCC2B08-8773-C547-9417-6D50A357579D}"/>
-    <hyperlink ref="C52" r:id="rId11" xr:uid="{4ED7AA7D-0161-9048-913F-4E262F489078}"/>
-    <hyperlink ref="C54" r:id="rId12" xr:uid="{D4B94815-2A3D-554A-9A3A-D6C41768932F}"/>
-    <hyperlink ref="C55" r:id="rId13" xr:uid="{B9A4BC97-C4E7-CB40-BDEE-3FC54B1A15F8}"/>
-    <hyperlink ref="C56" r:id="rId14" xr:uid="{1A254817-AA29-4349-9F3D-1F08E4B7BC6D}"/>
-    <hyperlink ref="C57" r:id="rId15" location="{Reaction_medium}Medium" xr:uid="{9FFFB41F-40DA-E844-8105-33FA71783875}"/>
-    <hyperlink ref="C58" r:id="rId16" location="{Operation_mode}Mode" xr:uid="{E49C1ABB-2410-D945-BAD5-E813751ECA22}"/>
-    <hyperlink ref="C73" r:id="rId17" location="{Light_source}LightSource" xr:uid="{5D5BAA03-A593-D246-AA1D-DD5A58EEB0FF}"/>
-    <hyperlink ref="C74" r:id="rId18" location="{Lamp}Lamp" xr:uid="{B474DE65-6CF2-6449-8CB9-C1A8F1227029}"/>
-    <hyperlink ref="C75" r:id="rId19" location="{Wavelength_nm}WL" xr:uid="{CDAAFAD0-E55A-C64F-A0E5-874107AAA07C}"/>
-    <hyperlink ref="C76" r:id="rId20" xr:uid="{D635B011-750E-414E-91E7-5327241CF37A}"/>
-    <hyperlink ref="C77:C78" r:id="rId21" display="http://w3id.org/solar/i/IlluminatedArea/{ID}" xr:uid="{4DFEDC35-DAA6-804C-B0F6-2CAF9BC91727}"/>
-    <hyperlink ref="C77" r:id="rId22" xr:uid="{1D48B95E-8BAD-E044-A7A5-74EFE823C221}"/>
-    <hyperlink ref="C78" r:id="rId23" xr:uid="{6118BC49-CEA9-7C4E-ABE8-63EA5ED604C9}"/>
-    <hyperlink ref="C49" r:id="rId24" xr:uid="{BD436ABE-9765-184F-AB49-2AAD056EA2AC}"/>
-    <hyperlink ref="C53" r:id="rId25" location="{Reactor_type}Reactor" xr:uid="{12796564-401A-904D-BA88-6DE0252945FE}"/>
-    <hyperlink ref="C60" r:id="rId26" xr:uid="{4A57F8C9-3F6B-F346-9C06-14ACCD76C291}"/>
-    <hyperlink ref="C59" r:id="rId27" xr:uid="{D05AEF8F-000B-5243-AA02-25149BFE83E8}"/>
+    <hyperlink ref="C36" r:id="rId1" xr:uid="{33CD0375-FDC4-864D-8BAE-CF58136577F6}"/>
+    <hyperlink ref="C37" r:id="rId2" xr:uid="{87955B5B-4B6D-4B4A-B115-3F447052E311}"/>
+    <hyperlink ref="C40" r:id="rId3" xr:uid="{3D40A9A3-79A8-4048-A619-0101D21BBBDB}"/>
+    <hyperlink ref="C38" r:id="rId4" xr:uid="{DF6AE900-F5E5-1A46-90FE-9B17C12CD5EA}"/>
+    <hyperlink ref="C39" r:id="rId5" xr:uid="{26286F07-CF01-3D4F-AF7E-24B1DFF4CAC5}"/>
+    <hyperlink ref="C41" r:id="rId6" xr:uid="{250FC759-8E91-AD4E-BB93-AAF3872DC404}"/>
+    <hyperlink ref="C43" r:id="rId7" xr:uid="{5D2E891D-0452-324E-AC63-3B5EB8FCC576}"/>
+    <hyperlink ref="C8" r:id="rId8" xr:uid="{B83A9430-8469-3340-8A32-6DDD9D53D7BD}"/>
+    <hyperlink ref="C9" r:id="rId9" xr:uid="{699A6F69-F379-0348-B5C9-C25D7DB140FB}"/>
+    <hyperlink ref="C44" r:id="rId10" xr:uid="{EFCC2B08-8773-C547-9417-6D50A357579D}"/>
+    <hyperlink ref="C45" r:id="rId11" xr:uid="{4ED7AA7D-0161-9048-913F-4E262F489078}"/>
+    <hyperlink ref="C47" r:id="rId12" xr:uid="{D4B94815-2A3D-554A-9A3A-D6C41768932F}"/>
+    <hyperlink ref="C48" r:id="rId13" xr:uid="{B9A4BC97-C4E7-CB40-BDEE-3FC54B1A15F8}"/>
+    <hyperlink ref="C49" r:id="rId14" xr:uid="{1A254817-AA29-4349-9F3D-1F08E4B7BC6D}"/>
+    <hyperlink ref="C50" r:id="rId15" location="{Reaction_medium}Medium" xr:uid="{9FFFB41F-40DA-E844-8105-33FA71783875}"/>
+    <hyperlink ref="C51" r:id="rId16" location="{Operation_mode}Mode" xr:uid="{E49C1ABB-2410-D945-BAD5-E813751ECA22}"/>
+    <hyperlink ref="C66" r:id="rId17" location="{Light_source}LightSource" xr:uid="{5D5BAA03-A593-D246-AA1D-DD5A58EEB0FF}"/>
+    <hyperlink ref="C67" r:id="rId18" location="{Lamp}Lamp" xr:uid="{B474DE65-6CF2-6449-8CB9-C1A8F1227029}"/>
+    <hyperlink ref="C68" r:id="rId19" location="{Wavelength_nm}WL" xr:uid="{CDAAFAD0-E55A-C64F-A0E5-874107AAA07C}"/>
+    <hyperlink ref="C69" r:id="rId20" xr:uid="{D635B011-750E-414E-91E7-5327241CF37A}"/>
+    <hyperlink ref="C70:C71" r:id="rId21" display="http://w3id.org/solar/i/IlluminatedArea/{ID}" xr:uid="{4DFEDC35-DAA6-804C-B0F6-2CAF9BC91727}"/>
+    <hyperlink ref="C70" r:id="rId22" xr:uid="{1D48B95E-8BAD-E044-A7A5-74EFE823C221}"/>
+    <hyperlink ref="C71" r:id="rId23" xr:uid="{6118BC49-CEA9-7C4E-ABE8-63EA5ED604C9}"/>
+    <hyperlink ref="C42" r:id="rId24" xr:uid="{BD436ABE-9765-184F-AB49-2AAD056EA2AC}"/>
+    <hyperlink ref="C46" r:id="rId25" location="{Reactor_type}Reactor" xr:uid="{12796564-401A-904D-BA88-6DE0252945FE}"/>
+    <hyperlink ref="C53" r:id="rId26" xr:uid="{4A57F8C9-3F6B-F346-9C06-14ACCD76C291}"/>
+    <hyperlink ref="C52" r:id="rId27" xr:uid="{D05AEF8F-000B-5243-AA02-25149BFE83E8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
queries to WD for chemicals
</commit_message>
<xml_diff>
--- a/knowledge-graph/mappings/solarchem-mapping.xlsx
+++ b/knowledge-graph/mappings/solarchem-mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aiglesias/GitHub/solarchem-ontology/knowledge-graph/mappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFC1055-417C-3D45-A69E-D5C00C4EADBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7507A4DA-ED0F-1741-B95D-6FA43BB7ACDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38420" yWindow="-1020" windowWidth="38400" windowHeight="21100" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-1020" windowWidth="38400" windowHeight="21100" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefix" sheetId="1" r:id="rId1"/>
@@ -1224,8 +1224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1764,7 +1764,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2079,8 +2079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
links to chemical concepts added
</commit_message>
<xml_diff>
--- a/knowledge-graph/mappings/solarchem-mapping.xlsx
+++ b/knowledge-graph/mappings/solarchem-mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aiglesias/GitHub/solarchem-ontology/knowledge-graph/mappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858C4802-BD44-EB41-91A3-04A28CCC09C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D773D556-730D-3348-8CEF-F7C56DB1FCFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="500" windowWidth="28740" windowHeight="17500" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
     <author>tc={16A91D93-63D0-AF4D-B9FC-79B454B39BC8}</author>
   </authors>
   <commentList>
-    <comment ref="B47" authorId="0" shapeId="0" xr:uid="{16A91D93-63D0-AF4D-B9FC-79B454B39BC8}">
+    <comment ref="B54" authorId="0" shapeId="0" xr:uid="{16A91D93-63D0-AF4D-B9FC-79B454B39BC8}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="230">
   <si>
     <t>Prefix</t>
   </si>
@@ -728,6 +728,24 @@
   </si>
   <si>
     <t>http://w3id.org/solar/i/Article/{No_de_Ref}</t>
+  </si>
+  <si>
+    <t>solar:hasChemical</t>
+  </si>
+  <si>
+    <t>CHEMICAL</t>
+  </si>
+  <si>
+    <t>{Chemicals}</t>
+  </si>
+  <si>
+    <t>{uri}</t>
+  </si>
+  <si>
+    <t>data/chemicals.csv</t>
+  </si>
+  <si>
+    <t>CO-CATALYST4</t>
   </si>
 </sst>
 </file>
@@ -1142,7 +1160,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="B47" dT="2024-03-23T15:13:35.29" personId="{38DFC2E4-73EA-D74C-967B-80CBA1CEA104}" id="{16A91D93-63D0-AF4D-B9FC-79B454B39BC8}">
+  <threadedComment ref="B54" dT="2024-03-23T15:13:35.29" personId="{38DFC2E4-73EA-D74C-967B-80CBA1CEA104}" id="{16A91D93-63D0-AF4D-B9FC-79B454B39BC8}">
     <text xml:space="preserve">No está en la onto, tiene valor especial con respecto al resto de inputs
 </text>
   </threadedComment>
@@ -1331,10 +1349,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView topLeftCell="A11" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1939,6 +1957,28 @@
         <v>38</v>
       </c>
     </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1950,7 +1990,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2246,6 +2286,14 @@
       </c>
       <c r="C26" s="8" t="s">
         <v>176</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>225</v>
+      </c>
+      <c r="C27" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -2287,10 +2335,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H90"/>
+  <dimension ref="A1:H99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54:A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2577,7 +2625,7 @@
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>48</v>
       </c>
@@ -2594,7 +2642,7 @@
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>48</v>
       </c>
@@ -2611,7 +2659,7 @@
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>48</v>
       </c>
@@ -2628,7 +2676,7 @@
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>48</v>
       </c>
@@ -2643,7 +2691,7 @@
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>48</v>
       </c>
@@ -2660,7 +2708,7 @@
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>48</v>
       </c>
@@ -2677,187 +2725,198 @@
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>102</v>
+        <v>48</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>79</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="C23" s="8"/>
+      <c r="D23" s="7"/>
       <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F23" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H23" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>102</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>103</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27" s="7"/>
+        <v>109</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>52</v>
+      </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>64</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>52</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="D28" s="7"/>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>64</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D30" s="7"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H31" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>80</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>79</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="D32" s="7"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D33" s="7"/>
+        <v>73</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -2865,36 +2924,42 @@
         <v>81</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>79</v>
+        <v>224</v>
+      </c>
+      <c r="C35" s="8"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H35" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>60</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="D36" s="7"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>50</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>52</v>
@@ -2902,13 +2967,13 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>65</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>79</v>
@@ -2916,360 +2981,388 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
-        <v>88</v>
+        <v>229</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>90</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="C39" s="8"/>
       <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H39" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>52</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="D40" s="7"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D42" s="7"/>
+        <v>69</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>52</v>
+        <v>224</v>
+      </c>
+      <c r="C43" s="8"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H43" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>79</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="D44" s="7"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
-        <v>164</v>
+        <v>88</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="D45" s="7"/>
+        <v>91</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
-        <v>164</v>
+        <v>88</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>166</v>
+        <v>92</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>164</v>
+        <v>88</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>79</v>
+        <v>224</v>
+      </c>
+      <c r="C47" s="8"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H47" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
-        <v>39</v>
+        <v>93</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F48" s="9"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="7"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D48" s="7"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
-        <v>39</v>
+        <v>93</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>76</v>
+        <v>50</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
-        <v>39</v>
+        <v>93</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>77</v>
+        <v>65</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>95</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
-        <v>39</v>
+        <v>93</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+      <c r="C51" s="8"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H51" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
-        <v>39</v>
+        <v>164</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D52" s="7"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
-        <v>39</v>
+        <v>164</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>78</v>
+        <v>50</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>166</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
-        <v>39</v>
+        <v>164</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>89</v>
+        <v>167</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>168</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+      <c r="F54" s="9"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
-        <v>39</v>
+        <v>164</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+      <c r="C55" s="8"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H55" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>46</v>
+        <v>173</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>169</v>
+        <v>223</v>
       </c>
       <c r="D56" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>112</v>
+        <v>46</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="D57" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>110</v>
+        <v>46</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>111</v>
+        <v>77</v>
       </c>
       <c r="D58" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>110</v>
+        <v>46</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>174</v>
+        <v>86</v>
       </c>
       <c r="D59" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>110</v>
+        <v>46</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>110</v>
+        <v>46</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>116</v>
+        <v>78</v>
       </c>
       <c r="D61" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>110</v>
+        <v>46</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="D62" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>110</v>
+        <v>46</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>139</v>
+        <v>97</v>
       </c>
       <c r="D63" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>110</v>
+        <v>46</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>140</v>
+        <v>169</v>
       </c>
       <c r="D64" s="7" t="s">
         <v>52</v>
@@ -3280,10 +3373,10 @@
         <v>39</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>175</v>
+        <v>113</v>
       </c>
       <c r="D65" s="7" t="s">
         <v>52</v>
@@ -3297,7 +3390,7 @@
         <v>110</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>176</v>
+        <v>111</v>
       </c>
       <c r="D66" s="7" t="s">
         <v>52</v>
@@ -3305,27 +3398,27 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
-        <v>118</v>
+        <v>39</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>128</v>
+        <v>110</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>174</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
-        <v>118</v>
+        <v>39</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>137</v>
+        <v>110</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>115</v>
       </c>
       <c r="D68" s="7" t="s">
         <v>52</v>
@@ -3333,27 +3426,27 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
-        <v>177</v>
+        <v>39</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C69" s="7" t="s">
-        <v>129</v>
+        <v>110</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>116</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="7" t="s">
-        <v>177</v>
+        <v>39</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C70" s="7" t="s">
-        <v>136</v>
+        <v>110</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>117</v>
       </c>
       <c r="D70" s="7" t="s">
         <v>52</v>
@@ -3361,27 +3454,27 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="s">
-        <v>178</v>
+        <v>39</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>179</v>
+        <v>110</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>139</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
-        <v>178</v>
+        <v>39</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>180</v>
+        <v>110</v>
+      </c>
+      <c r="C72" s="8" t="s">
+        <v>140</v>
       </c>
       <c r="D72" s="7" t="s">
         <v>52</v>
@@ -3389,27 +3482,27 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="7" t="s">
-        <v>120</v>
+        <v>39</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>130</v>
+        <v>110</v>
+      </c>
+      <c r="C73" s="8" t="s">
+        <v>175</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="7" t="s">
-        <v>120</v>
+        <v>39</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>134</v>
+        <v>110</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>176</v>
       </c>
       <c r="D74" s="7" t="s">
         <v>52</v>
@@ -3417,13 +3510,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B75" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D75" s="7" t="s">
         <v>79</v>
@@ -3431,13 +3524,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B76" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D76" s="7" t="s">
         <v>52</v>
@@ -3445,13 +3538,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="s">
-        <v>122</v>
+        <v>177</v>
       </c>
       <c r="B77" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D77" s="7" t="s">
         <v>79</v>
@@ -3459,13 +3552,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="7" t="s">
-        <v>122</v>
+        <v>177</v>
       </c>
       <c r="B78" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D78" s="7" t="s">
         <v>52</v>
@@ -3473,27 +3566,27 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="s">
-        <v>141</v>
+        <v>178</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="C79" s="8" t="s">
-        <v>145</v>
+        <v>55</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>179</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="7" t="s">
-        <v>141</v>
+        <v>178</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="C80" s="8" t="s">
-        <v>147</v>
+        <v>57</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>180</v>
       </c>
       <c r="D80" s="7" t="s">
         <v>52</v>
@@ -3501,27 +3594,27 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="7" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="C81" s="8" t="s">
-        <v>152</v>
+        <v>55</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>130</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="7" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="C82" s="8" t="s">
-        <v>153</v>
+        <v>57</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>134</v>
       </c>
       <c r="D82" s="7" t="s">
         <v>52</v>
@@ -3529,27 +3622,27 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="7" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="C83" s="8" t="s">
-        <v>154</v>
+        <v>55</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="D83" s="7" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="C84" s="8" t="s">
-        <v>155</v>
+        <v>57</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>135</v>
       </c>
       <c r="D84" s="7" t="s">
         <v>52</v>
@@ -3557,13 +3650,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="s">
-        <v>156</v>
+        <v>122</v>
       </c>
       <c r="B85" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>160</v>
+        <v>132</v>
       </c>
       <c r="D85" s="7" t="s">
         <v>79</v>
@@ -3571,13 +3664,13 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
-        <v>156</v>
+        <v>122</v>
       </c>
       <c r="B86" s="7" t="s">
         <v>57</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>162</v>
+        <v>133</v>
       </c>
       <c r="D86" s="7" t="s">
         <v>52</v>
@@ -3585,27 +3678,27 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C87" s="7" t="s">
-        <v>161</v>
+        <v>138</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>145</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C88" s="7" t="s">
-        <v>163</v>
+        <v>146</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>147</v>
       </c>
       <c r="D88" s="7" t="s">
         <v>52</v>
@@ -3613,66 +3706,189 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="7" t="s">
-        <v>171</v>
+        <v>141</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C89" s="7" t="s">
-        <v>170</v>
+        <v>148</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>152</v>
       </c>
       <c r="D89" s="7" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C90" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D90" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C91" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D91" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D92" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="B94" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="D94" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D95" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B96" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="D96" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="B90" s="7" t="s">
+      <c r="B97" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C97" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="D97" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B98" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C90" s="7" t="s">
+      <c r="C98" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="D90" s="7" t="s">
-        <v>52</v>
+      <c r="D98" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>226</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C49" r:id="rId1" xr:uid="{33CD0375-FDC4-864D-8BAE-CF58136577F6}"/>
-    <hyperlink ref="C50" r:id="rId2" xr:uid="{87955B5B-4B6D-4B4A-B115-3F447052E311}"/>
-    <hyperlink ref="C53" r:id="rId3" xr:uid="{3D40A9A3-79A8-4048-A619-0101D21BBBDB}"/>
-    <hyperlink ref="C51" r:id="rId4" xr:uid="{DF6AE900-F5E5-1A46-90FE-9B17C12CD5EA}"/>
-    <hyperlink ref="C52" r:id="rId5" xr:uid="{26286F07-CF01-3D4F-AF7E-24B1DFF4CAC5}"/>
-    <hyperlink ref="C54" r:id="rId6" xr:uid="{250FC759-8E91-AD4E-BB93-AAF3872DC404}"/>
-    <hyperlink ref="C56" r:id="rId7" xr:uid="{5D2E891D-0452-324E-AC63-3B5EB8FCC576}"/>
+    <hyperlink ref="C57" r:id="rId1" xr:uid="{33CD0375-FDC4-864D-8BAE-CF58136577F6}"/>
+    <hyperlink ref="C58" r:id="rId2" xr:uid="{87955B5B-4B6D-4B4A-B115-3F447052E311}"/>
+    <hyperlink ref="C61" r:id="rId3" xr:uid="{3D40A9A3-79A8-4048-A619-0101D21BBBDB}"/>
+    <hyperlink ref="C59" r:id="rId4" xr:uid="{DF6AE900-F5E5-1A46-90FE-9B17C12CD5EA}"/>
+    <hyperlink ref="C60" r:id="rId5" xr:uid="{26286F07-CF01-3D4F-AF7E-24B1DFF4CAC5}"/>
+    <hyperlink ref="C62" r:id="rId6" xr:uid="{250FC759-8E91-AD4E-BB93-AAF3872DC404}"/>
+    <hyperlink ref="C64" r:id="rId7" xr:uid="{5D2E891D-0452-324E-AC63-3B5EB8FCC576}"/>
     <hyperlink ref="C21" r:id="rId8" xr:uid="{B83A9430-8469-3340-8A32-6DDD9D53D7BD}"/>
     <hyperlink ref="C22" r:id="rId9" xr:uid="{699A6F69-F379-0348-B5C9-C25D7DB140FB}"/>
-    <hyperlink ref="C57" r:id="rId10" xr:uid="{EFCC2B08-8773-C547-9417-6D50A357579D}"/>
-    <hyperlink ref="C58" r:id="rId11" xr:uid="{4ED7AA7D-0161-9048-913F-4E262F489078}"/>
-    <hyperlink ref="C60" r:id="rId12" xr:uid="{D4B94815-2A3D-554A-9A3A-D6C41768932F}"/>
-    <hyperlink ref="C61" r:id="rId13" xr:uid="{B9A4BC97-C4E7-CB40-BDEE-3FC54B1A15F8}"/>
-    <hyperlink ref="C62" r:id="rId14" xr:uid="{1A254817-AA29-4349-9F3D-1F08E4B7BC6D}"/>
-    <hyperlink ref="C63" r:id="rId15" location="{Reaction_medium}Medium" xr:uid="{9FFFB41F-40DA-E844-8105-33FA71783875}"/>
-    <hyperlink ref="C64" r:id="rId16" location="{Operation_mode}Mode" xr:uid="{E49C1ABB-2410-D945-BAD5-E813751ECA22}"/>
-    <hyperlink ref="C79" r:id="rId17" location="{Light_source}LightSource" xr:uid="{5D5BAA03-A593-D246-AA1D-DD5A58EEB0FF}"/>
-    <hyperlink ref="C80" r:id="rId18" location="{Lamp}Lamp" xr:uid="{B474DE65-6CF2-6449-8CB9-C1A8F1227029}"/>
-    <hyperlink ref="C81" r:id="rId19" location="{Wavelength_nm}WL" xr:uid="{CDAAFAD0-E55A-C64F-A0E5-874107AAA07C}"/>
-    <hyperlink ref="C82" r:id="rId20" xr:uid="{D635B011-750E-414E-91E7-5327241CF37A}"/>
-    <hyperlink ref="C83:C84" r:id="rId21" display="http://w3id.org/solar/i/IlluminatedArea/{ID}" xr:uid="{4DFEDC35-DAA6-804C-B0F6-2CAF9BC91727}"/>
-    <hyperlink ref="C83" r:id="rId22" xr:uid="{1D48B95E-8BAD-E044-A7A5-74EFE823C221}"/>
-    <hyperlink ref="C84" r:id="rId23" xr:uid="{6118BC49-CEA9-7C4E-ABE8-63EA5ED604C9}"/>
-    <hyperlink ref="C55" r:id="rId24" xr:uid="{BD436ABE-9765-184F-AB49-2AAD056EA2AC}"/>
-    <hyperlink ref="C59" r:id="rId25" location="{Reactor_type}Reactor" xr:uid="{12796564-401A-904D-BA88-6DE0252945FE}"/>
-    <hyperlink ref="C66" r:id="rId26" xr:uid="{4A57F8C9-3F6B-F346-9C06-14ACCD76C291}"/>
-    <hyperlink ref="C65" r:id="rId27" xr:uid="{D05AEF8F-000B-5243-AA02-25149BFE83E8}"/>
+    <hyperlink ref="C65" r:id="rId10" xr:uid="{EFCC2B08-8773-C547-9417-6D50A357579D}"/>
+    <hyperlink ref="C66" r:id="rId11" xr:uid="{4ED7AA7D-0161-9048-913F-4E262F489078}"/>
+    <hyperlink ref="C68" r:id="rId12" xr:uid="{D4B94815-2A3D-554A-9A3A-D6C41768932F}"/>
+    <hyperlink ref="C69" r:id="rId13" xr:uid="{B9A4BC97-C4E7-CB40-BDEE-3FC54B1A15F8}"/>
+    <hyperlink ref="C70" r:id="rId14" xr:uid="{1A254817-AA29-4349-9F3D-1F08E4B7BC6D}"/>
+    <hyperlink ref="C71" r:id="rId15" location="{Reaction_medium}Medium" xr:uid="{9FFFB41F-40DA-E844-8105-33FA71783875}"/>
+    <hyperlink ref="C72" r:id="rId16" location="{Operation_mode}Mode" xr:uid="{E49C1ABB-2410-D945-BAD5-E813751ECA22}"/>
+    <hyperlink ref="C87" r:id="rId17" location="{Light_source}LightSource" xr:uid="{5D5BAA03-A593-D246-AA1D-DD5A58EEB0FF}"/>
+    <hyperlink ref="C88" r:id="rId18" location="{Lamp}Lamp" xr:uid="{B474DE65-6CF2-6449-8CB9-C1A8F1227029}"/>
+    <hyperlink ref="C89" r:id="rId19" location="{Wavelength_nm}WL" xr:uid="{CDAAFAD0-E55A-C64F-A0E5-874107AAA07C}"/>
+    <hyperlink ref="C90" r:id="rId20" xr:uid="{D635B011-750E-414E-91E7-5327241CF37A}"/>
+    <hyperlink ref="C91:C92" r:id="rId21" display="http://w3id.org/solar/i/IlluminatedArea/{ID}" xr:uid="{4DFEDC35-DAA6-804C-B0F6-2CAF9BC91727}"/>
+    <hyperlink ref="C91" r:id="rId22" xr:uid="{1D48B95E-8BAD-E044-A7A5-74EFE823C221}"/>
+    <hyperlink ref="C92" r:id="rId23" xr:uid="{6118BC49-CEA9-7C4E-ABE8-63EA5ED604C9}"/>
+    <hyperlink ref="C63" r:id="rId24" xr:uid="{BD436ABE-9765-184F-AB49-2AAD056EA2AC}"/>
+    <hyperlink ref="C67" r:id="rId25" location="{Reactor_type}Reactor" xr:uid="{12796564-401A-904D-BA88-6DE0252945FE}"/>
+    <hyperlink ref="C74" r:id="rId26" xr:uid="{4A57F8C9-3F6B-F346-9C06-14ACCD76C291}"/>
+    <hyperlink ref="C73" r:id="rId27" xr:uid="{D05AEF8F-000B-5243-AA02-25149BFE83E8}"/>
     <hyperlink ref="C15" r:id="rId28" xr:uid="{2503A0AF-6306-B442-BAF4-FE5558F49054}"/>
     <hyperlink ref="C13" r:id="rId29" xr:uid="{43608D61-A942-0444-9531-A10AB9261A99}"/>
     <hyperlink ref="C10" r:id="rId30" xr:uid="{4A64E9B0-01B7-7B4D-9DDC-33AFEBA4C9E6}"/>
-    <hyperlink ref="C48" r:id="rId31" xr:uid="{590C6980-47B5-A946-AD9A-4A310BA4F056}"/>
+    <hyperlink ref="C56" r:id="rId31" xr:uid="{590C6980-47B5-A946-AD9A-4A310BA4F056}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
fixing little mistakes and https for w3id
</commit_message>
<xml_diff>
--- a/knowledge-graph/mappings/solarchem-mapping.xlsx
+++ b/knowledge-graph/mappings/solarchem-mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aiglesias/GitHub/solarchem-ontology/knowledge-graph/mappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D773D556-730D-3348-8CEF-F7C56DB1FCFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCEC3420-F934-CE47-B86A-D4BB8DA2D8F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="28740" windowHeight="17500" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28740" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefix" sheetId="1" r:id="rId1"/>
@@ -136,9 +136,6 @@
     <t>https://schema.org/</t>
   </si>
   <si>
-    <t>http://w3id.org/solar/i/</t>
-  </si>
-  <si>
     <t>solar</t>
   </si>
   <si>
@@ -148,18 +145,6 @@
     <t>solarpec</t>
   </si>
   <si>
-    <t>http://w3id.org/solar/o/core#</t>
-  </si>
-  <si>
-    <t>http://w3id.org/solar/o/ec#</t>
-  </si>
-  <si>
-    <t>http://w3id.org/solar/o/pec#</t>
-  </si>
-  <si>
-    <t>http://w3id.org/solar/o/pc#</t>
-  </si>
-  <si>
     <t>ARTICLE</t>
   </si>
   <si>
@@ -199,9 +184,6 @@
     <t>prov:used</t>
   </si>
   <si>
-    <t>http://w3id.org/solar/i/ExpExec/{ID}</t>
-  </si>
-  <si>
     <t>CATALYST</t>
   </si>
   <si>
@@ -286,15 +268,6 @@
     <t>solarpc</t>
   </si>
   <si>
-    <t>http://w3id.org/solar/i/Input/Catalyst/{ID}-{Catalyst}</t>
-  </si>
-  <si>
-    <t>http://w3id.org/solar/i/Input/Co-catalyst/{ID}-{Co_catalyst}</t>
-  </si>
-  <si>
-    <t>http://w3id.org/solar/i/Input/Support/{ID}-{Support}</t>
-  </si>
-  <si>
     <t>float</t>
   </si>
   <si>
@@ -316,18 +289,9 @@
     <t>{percent_cc_3}</t>
   </si>
   <si>
-    <t>http://w3id.org/solar/i/Input/Co-catalyst/{ID}-{co_catalyst_2}</t>
-  </si>
-  <si>
-    <t>http://w3id.org/solar/i/Input/Co-catalyst/{ID}-{co_catalyst_3}</t>
-  </si>
-  <si>
     <t>DOPANT</t>
   </si>
   <si>
-    <t>http://w3id.org/solar/i/Input/Dopant/{ID}-{Dopant}</t>
-  </si>
-  <si>
     <t>{Dopant}</t>
   </si>
   <si>
@@ -349,21 +313,12 @@
     <t>{Dyes}</t>
   </si>
   <si>
-    <t>http://w3id.org/solar/i/Input/Dye/{ID}-{Dyes}</t>
-  </si>
-  <si>
     <t>solar:hasBandGap</t>
   </si>
   <si>
     <t>solar:hasSurfaceArea</t>
   </si>
   <si>
-    <t>http://w3id.org/solar/i/SurfaceArea/{ID}-{Catalyst}</t>
-  </si>
-  <si>
-    <t>http://w3id.org/solar/i/BandGap/{ID}-{Catalyst}</t>
-  </si>
-  <si>
     <t>BANDGAP</t>
   </si>
   <si>
@@ -391,27 +346,9 @@
     <t>solar:hasCondition</t>
   </si>
   <si>
-    <t>http://w3id.org/solar/i/Condition/pH/{ID}</t>
-  </si>
-  <si>
     <t>solar:hasLightSource</t>
   </si>
   <si>
-    <t>http://w3id.org/solar/i/Condition/LightSource/{ID}</t>
-  </si>
-  <si>
-    <t>http://w3id.org/solar/i/Condition/Reactor/{ID}</t>
-  </si>
-  <si>
-    <t>http://w3id.org/solar/i/Condition/Pressure/{ID}</t>
-  </si>
-  <si>
-    <t>http://w3id.org/solar/i/Condition/Temperature/{ID}</t>
-  </si>
-  <si>
-    <t>http://w3id.org/solar/i/Condition/Time/{ID}</t>
-  </si>
-  <si>
     <t>PH</t>
   </si>
   <si>
@@ -430,9 +367,6 @@
     <t>solar:pHCondition</t>
   </si>
   <si>
-    <t>solarpc:ReactorCondition</t>
-  </si>
-  <si>
     <t>solar:PressureCondition</t>
   </si>
   <si>
@@ -475,12 +409,6 @@
     <t>rdf:type</t>
   </si>
   <si>
-    <t>http://w3id.org/solar/o/core#{Reaction_medium}Medium</t>
-  </si>
-  <si>
-    <t>http://w3id.org/solar/o/core#{Operation_mode}Mode</t>
-  </si>
-  <si>
     <t>LIGHT</t>
   </si>
   <si>
@@ -493,15 +421,9 @@
     <t>obi:0400065</t>
   </si>
   <si>
-    <t>http://w3id.org/solar/o/core#{Light_source}LightSource</t>
-  </si>
-  <si>
     <t>solar:hasLamp</t>
   </si>
   <si>
-    <t>http://w3id.org/solar/o/core#{Lamp}Lamp</t>
-  </si>
-  <si>
     <t>solar:hasWavelength</t>
   </si>
   <si>
@@ -514,18 +436,6 @@
     <t>solar:hasIlluminatedArea</t>
   </si>
   <si>
-    <t>http://w3id.org/solar/o/core#{Wavelength_nm}WL</t>
-  </si>
-  <si>
-    <t>http://w3id.org/solar/i/IlluminatedArea/{ID}</t>
-  </si>
-  <si>
-    <t>http://w3id.org/solar/i/Power/{ID}</t>
-  </si>
-  <si>
-    <t>http://w3id.org/solar/i/Irradiance/{ID}</t>
-  </si>
-  <si>
     <t>POWER</t>
   </si>
   <si>
@@ -565,9 +475,6 @@
     <t>{CO2_H2O_reductant_ratio}</t>
   </si>
   <si>
-    <t>http://w3id.org/solar/i/Input/Reductant/{ID}-{Reductant}</t>
-  </si>
-  <si>
     <t>{Illuminated_area_m2}</t>
   </si>
   <si>
@@ -580,15 +487,6 @@
     <t>solar:reportedIn</t>
   </si>
   <si>
-    <t>http://w3id.org/solar/o/core#{Reactor_type}Reactor</t>
-  </si>
-  <si>
-    <t>http://w3id.org/solar/i/Condition/ReactorVolume/{ID}</t>
-  </si>
-  <si>
-    <t>http://w3id.org/solar/i/Condition/ReactorResidenceTime/{ID}</t>
-  </si>
-  <si>
     <t>REACTORVOL</t>
   </si>
   <si>
@@ -631,9 +529,6 @@
     <t>{title}</t>
   </si>
   <si>
-    <t>schema:issueNumer</t>
-  </si>
-  <si>
     <t>{biblio.issue}</t>
   </si>
   <si>
@@ -667,9 +562,6 @@
     <t>schema:author</t>
   </si>
   <si>
-    <t>http://w3id.org/solar/i/Author/{authorships.author.orcid}</t>
-  </si>
-  <si>
     <t>{solar_id}</t>
   </si>
   <si>
@@ -682,9 +574,6 @@
     <t>schema:affiliation</t>
   </si>
   <si>
-    <t>http://w3id.org/solar/i/Affiliation/{institutions.id}</t>
-  </si>
-  <si>
     <t>AFFILIATION</t>
   </si>
   <si>
@@ -694,21 +583,12 @@
     <t>schema:addressCountry</t>
   </si>
   <si>
-    <t>http://w3id.org/solar/i/Country/{institutions.country_code}</t>
-  </si>
-  <si>
     <t>schema:Person</t>
   </si>
   <si>
-    <t>http://w3id.org/solar/i/Author/{author.orcid}</t>
-  </si>
-  <si>
     <t>schema:Organization</t>
   </si>
   <si>
-    <t>http://w3id.org/solar/i/Article/{solar_id}</t>
-  </si>
-  <si>
     <t>schema:ScholarlyArticle</t>
   </si>
   <si>
@@ -721,15 +601,6 @@
     <t>iterator</t>
   </si>
   <si>
-    <t>"$[*]"</t>
-  </si>
-  <si>
-    <t>"$[*].authorships[*]"</t>
-  </si>
-  <si>
-    <t>http://w3id.org/solar/i/Article/{No_de_Ref}</t>
-  </si>
-  <si>
     <t>solar:hasChemical</t>
   </si>
   <si>
@@ -746,6 +617,135 @@
   </si>
   <si>
     <t>CO-CATALYST4</t>
+  </si>
+  <si>
+    <t>$[*]</t>
+  </si>
+  <si>
+    <t>$[*].authorships[*]</t>
+  </si>
+  <si>
+    <t>schema:issueNumber</t>
+  </si>
+  <si>
+    <t>solar:ReactorCondition</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/o/core#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/o/ec#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/o/pec#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/o/pc#</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/o/core#{Reactor_type}Reactor</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/o/core#{Reaction_medium}Medium</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/o/core#{Operation_mode}Mode</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/o/core#{Light_source}LightSource</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/o/core#{Lamp}Lamp</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/o/core#{Wavelength_nm}WL</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/i/</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/i/Article/{solar_id}</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/i/Author/{author.orcid}</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/i/Affiliation/{institutions.id}</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/i/ExpExec/{ID}</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/i/Input/Catalyst/{ID}-{Catalyst}</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/i/BandGap/{ID}-{Catalyst}</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/i/SurfaceArea/{ID}-{Catalyst}</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/i/Input/Co-catalyst/{ID}-{Co_catalyst}</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/i/Input/Co-catalyst/{ID}-{co_catalyst_2}</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/i/Input/Co-catalyst/{ID}-{co_catalyst_3}</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/i/Input/Support/{ID}-{Support}</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/i/Input/Dopant/{ID}-{Dopant}</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/i/Input/Dye/{ID}-{Dyes}</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/i/Input/Reductant/{ID}-{Reductant}</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/i/Condition/pH/{ID}</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/i/Condition/Reactor/{ID}</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/i/Condition/Pressure/{ID}</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/i/Condition/Temperature/{ID}</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/i/Condition/Time/{ID}</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/i/Condition/LightSource/{ID}</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/i/Power/{ID}</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/i/Irradiance/{ID}</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/i/IlluminatedArea/{ID}</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/i/Condition/ReactorVolume/{ID}</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/i/Condition/ReactorResidenceTime/{ID}</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/i/Author/{authorships.author.orcid}</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/i/Country/{institutions.country_code}</t>
+  </si>
+  <si>
+    <t>https://w3id.org/solar/i/Article/{No_de_Ref}</t>
   </si>
 </sst>
 </file>
@@ -1171,8 +1171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1240,74 +1240,74 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>30</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>31</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>32</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>33</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>183</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1315,7 +1315,7 @@
         <v>23</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>26</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -1326,7 +1326,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B17" r:id="rId1" xr:uid="{F8754CBA-ECDB-4444-8F8F-EBA6BEFBBCF3}"/>
+    <hyperlink ref="B17" r:id="rId1" display="http://w3id.org/solar/i/" xr:uid="{F8754CBA-ECDB-4444-8F8F-EBA6BEFBBCF3}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{4E1D75EA-0423-7E40-BBCD-B6BD079FA83E}"/>
     <hyperlink ref="B3" r:id="rId3" xr:uid="{D60B0DDB-58EA-FA48-A2CD-CBE7C55549A6}"/>
     <hyperlink ref="B4" r:id="rId4" xr:uid="{E6258B07-1D09-D64E-8845-A7B81A5A2C61}"/>
@@ -1351,8 +1351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1376,607 +1376,607 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>218</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>219</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>220</v>
+        <v>180</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>221</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>205</v>
+        <v>169</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>218</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>205</v>
+        <v>169</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>219</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>205</v>
+        <v>169</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>220</v>
+        <v>180</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>222</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>209</v>
+        <v>172</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>218</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>209</v>
+        <v>172</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>219</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>209</v>
+        <v>172</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>220</v>
+        <v>180</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>222</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>164</v>
+        <v>134</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>164</v>
+        <v>134</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
-        <v>156</v>
+        <v>126</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
-        <v>156</v>
+        <v>126</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>157</v>
+        <v>127</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
-        <v>157</v>
+        <v>127</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
-        <v>225</v>
+        <v>182</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>228</v>
+        <v>185</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
-        <v>225</v>
+        <v>182</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1990,7 +1990,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2015,285 +2015,285 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>217</v>
+        <v>177</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>205</v>
+        <v>169</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>213</v>
+        <v>175</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>209</v>
+        <v>172</v>
       </c>
       <c r="B4" t="s">
-        <v>215</v>
+        <v>176</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>44</v>
-      </c>
       <c r="C5" s="8" t="s">
-        <v>47</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>76</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="B7" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>101</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>100</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>77</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>86</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>87</v>
+        <v>211</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>78</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>89</v>
+        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>97</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>164</v>
+        <v>134</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>169</v>
+        <v>215</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="B16" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>111</v>
+        <v>216</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="B17" t="s">
-        <v>124</v>
+        <v>190</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>114</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="B18" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>115</v>
+        <v>218</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="B19" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>116</v>
+        <v>219</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="B20" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>117</v>
+        <v>220</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="B21" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>113</v>
+        <v>221</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>156</v>
+        <v>126</v>
       </c>
       <c r="B22" t="s">
-        <v>158</v>
+        <v>128</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>154</v>
+        <v>222</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>157</v>
+        <v>127</v>
       </c>
       <c r="B23" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>155</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
       <c r="B24" t="s">
-        <v>172</v>
+        <v>141</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>153</v>
+        <v>224</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="B25" t="s">
-        <v>182</v>
+        <v>148</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>175</v>
+        <v>225</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
       <c r="B26" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>176</v>
+        <v>226</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>225</v>
+        <v>182</v>
       </c>
       <c r="C27" t="s">
-        <v>227</v>
+        <v>184</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -2302,31 +2302,31 @@
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" xr:uid="{329341A0-A072-9242-8F6F-A7B5E8616EED}"/>
-    <hyperlink ref="C6" r:id="rId2" xr:uid="{02AE9908-CF19-CB41-8387-762706A65FB6}"/>
-    <hyperlink ref="C9" r:id="rId3" xr:uid="{4B69325E-4848-5C4A-97E8-083D91448168}"/>
-    <hyperlink ref="C12" r:id="rId4" xr:uid="{6EF885FD-DCB7-D742-A7EE-E1398ABBDE76}"/>
-    <hyperlink ref="C10" r:id="rId5" xr:uid="{E84559C3-422D-E949-A0E2-77EA15D80EEC}"/>
-    <hyperlink ref="C11" r:id="rId6" xr:uid="{A141179C-E949-524D-B44F-359B38E10D12}"/>
-    <hyperlink ref="C13" r:id="rId7" xr:uid="{FD31A938-338A-0349-B696-E419DD58C7DB}"/>
-    <hyperlink ref="C14" r:id="rId8" xr:uid="{8614587D-753C-C145-A81C-DA020E193AD7}"/>
-    <hyperlink ref="C7" r:id="rId9" xr:uid="{A9E9C9C6-B4B7-7B45-B322-7FED04CC7F6F}"/>
-    <hyperlink ref="C8" r:id="rId10" xr:uid="{0B8F8956-6FC1-7148-8FCF-BD724E0E6194}"/>
-    <hyperlink ref="C16" r:id="rId11" xr:uid="{DB791FD6-560D-BC4B-95CF-C462CC61462D}"/>
-    <hyperlink ref="C17" r:id="rId12" xr:uid="{9CDFBDF7-DF8A-F247-9234-17EC239F807D}"/>
-    <hyperlink ref="C18" r:id="rId13" xr:uid="{765CBB11-AA14-E145-8CC6-3063571D0F24}"/>
-    <hyperlink ref="C19" r:id="rId14" xr:uid="{2CA5367A-ADF2-3948-A151-F9ED43232B41}"/>
-    <hyperlink ref="C20" r:id="rId15" xr:uid="{AF45DD89-DCAB-9D47-82E7-E1514F724422}"/>
-    <hyperlink ref="C21" r:id="rId16" xr:uid="{C6281ADE-B007-FF43-987D-BC199502F4A9}"/>
-    <hyperlink ref="C22" r:id="rId17" xr:uid="{809DAE46-CFDD-1347-93E9-73C62A907742}"/>
-    <hyperlink ref="C24" r:id="rId18" xr:uid="{A8085152-3BE9-844F-BD28-D23B3F3D0675}"/>
-    <hyperlink ref="C15" r:id="rId19" xr:uid="{CA6E68C4-20B1-9248-AA29-D1A87184FF3B}"/>
-    <hyperlink ref="C23" r:id="rId20" xr:uid="{215F075C-705C-D340-8B34-205253A7FE6F}"/>
-    <hyperlink ref="C26" r:id="rId21" xr:uid="{B26AE112-ECB2-9A41-AAD1-982D7EA177FD}"/>
-    <hyperlink ref="C25" r:id="rId22" xr:uid="{3EC1BB91-66EF-C94B-8ED5-9415761E18F4}"/>
-    <hyperlink ref="C3" r:id="rId23" xr:uid="{DEDE6565-8AF0-AF40-AC0A-D968929C048B}"/>
-    <hyperlink ref="C4" r:id="rId24" xr:uid="{3C93540B-86B3-724A-B86F-760806B53347}"/>
-    <hyperlink ref="C2" r:id="rId25" xr:uid="{9E514B95-A162-1546-9B35-1B705B10BD40}"/>
+    <hyperlink ref="C5" r:id="rId1" display="http://w3id.org/solar/i/ExpExec/{ID}" xr:uid="{329341A0-A072-9242-8F6F-A7B5E8616EED}"/>
+    <hyperlink ref="C6" r:id="rId2" display="http://w3id.org/solar/i/Input/Catalyst/{ID}-{Catalyst}" xr:uid="{02AE9908-CF19-CB41-8387-762706A65FB6}"/>
+    <hyperlink ref="C9" r:id="rId3" display="http://w3id.org/solar/i/Input/Co-catalyst/{ID}-{Co_catalyst}" xr:uid="{4B69325E-4848-5C4A-97E8-083D91448168}"/>
+    <hyperlink ref="C12" r:id="rId4" display="http://w3id.org/solar/i/Input/Support/{ID}-{Support}" xr:uid="{6EF885FD-DCB7-D742-A7EE-E1398ABBDE76}"/>
+    <hyperlink ref="C10" r:id="rId5" display="http://w3id.org/solar/i/Input/Co-catalyst/{ID}-{co_catalyst_2}" xr:uid="{E84559C3-422D-E949-A0E2-77EA15D80EEC}"/>
+    <hyperlink ref="C11" r:id="rId6" display="http://w3id.org/solar/i/Input/Co-catalyst/{ID}-{co_catalyst_3}" xr:uid="{A141179C-E949-524D-B44F-359B38E10D12}"/>
+    <hyperlink ref="C13" r:id="rId7" display="http://w3id.org/solar/i/Input/Dopant/{ID}-{Dopant}" xr:uid="{FD31A938-338A-0349-B696-E419DD58C7DB}"/>
+    <hyperlink ref="C14" r:id="rId8" display="http://w3id.org/solar/i/Input/Dye/{ID}-{Dyes}" xr:uid="{8614587D-753C-C145-A81C-DA020E193AD7}"/>
+    <hyperlink ref="C7" r:id="rId9" display="http://w3id.org/solar/i/BandGap/{ID}-{Catalyst}" xr:uid="{A9E9C9C6-B4B7-7B45-B322-7FED04CC7F6F}"/>
+    <hyperlink ref="C8" r:id="rId10" display="http://w3id.org/solar/i/SurfaceArea/{ID}-{Catalyst}" xr:uid="{0B8F8956-6FC1-7148-8FCF-BD724E0E6194}"/>
+    <hyperlink ref="C16" r:id="rId11" display="http://w3id.org/solar/i/Condition/pH/{ID}" xr:uid="{DB791FD6-560D-BC4B-95CF-C462CC61462D}"/>
+    <hyperlink ref="C17" r:id="rId12" display="http://w3id.org/solar/i/Condition/Reactor/{ID}" xr:uid="{9CDFBDF7-DF8A-F247-9234-17EC239F807D}"/>
+    <hyperlink ref="C18" r:id="rId13" display="http://w3id.org/solar/i/Condition/Pressure/{ID}" xr:uid="{765CBB11-AA14-E145-8CC6-3063571D0F24}"/>
+    <hyperlink ref="C19" r:id="rId14" display="http://w3id.org/solar/i/Condition/Temperature/{ID}" xr:uid="{2CA5367A-ADF2-3948-A151-F9ED43232B41}"/>
+    <hyperlink ref="C20" r:id="rId15" display="http://w3id.org/solar/i/Condition/Time/{ID}" xr:uid="{AF45DD89-DCAB-9D47-82E7-E1514F724422}"/>
+    <hyperlink ref="C21" r:id="rId16" display="http://w3id.org/solar/i/Condition/LightSource/{ID}" xr:uid="{C6281ADE-B007-FF43-987D-BC199502F4A9}"/>
+    <hyperlink ref="C22" r:id="rId17" display="http://w3id.org/solar/i/Power/{ID}" xr:uid="{809DAE46-CFDD-1347-93E9-73C62A907742}"/>
+    <hyperlink ref="C24" r:id="rId18" display="http://w3id.org/solar/i/IlluminatedArea/{ID}" xr:uid="{A8085152-3BE9-844F-BD28-D23B3F3D0675}"/>
+    <hyperlink ref="C15" r:id="rId19" display="http://w3id.org/solar/i/Input/Reductant/{ID}-{Reductant}" xr:uid="{CA6E68C4-20B1-9248-AA29-D1A87184FF3B}"/>
+    <hyperlink ref="C23" r:id="rId20" display="http://w3id.org/solar/i/Irradiance/{ID}" xr:uid="{215F075C-705C-D340-8B34-205253A7FE6F}"/>
+    <hyperlink ref="C26" r:id="rId21" display="http://w3id.org/solar/i/Condition/ReactorResidenceTime/{ID}" xr:uid="{B26AE112-ECB2-9A41-AAD1-982D7EA177FD}"/>
+    <hyperlink ref="C25" r:id="rId22" display="http://w3id.org/solar/i/Condition/ReactorVolume/{ID}" xr:uid="{3EC1BB91-66EF-C94B-8ED5-9415761E18F4}"/>
+    <hyperlink ref="C3" r:id="rId23" display="http://w3id.org/solar/i/Author/{author.orcid}" xr:uid="{DEDE6565-8AF0-AF40-AC0A-D968929C048B}"/>
+    <hyperlink ref="C4" r:id="rId24" display="http://w3id.org/solar/i/Affiliation/{institutions.id}" xr:uid="{3C93540B-86B3-724A-B86F-760806B53347}"/>
+    <hyperlink ref="C2" r:id="rId25" display="http://w3id.org/solar/i/Article/{solar_id}" xr:uid="{9E514B95-A162-1546-9B35-1B705B10BD40}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2337,8 +2337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:A55"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2366,7 +2366,7 @@
         <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>14</v>
@@ -2380,13 +2380,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>185</v>
+        <v>151</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>186</v>
+        <v>152</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="1"/>
@@ -2396,13 +2396,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>187</v>
+        <v>153</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>188</v>
+        <v>154</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="1"/>
@@ -2412,13 +2412,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>189</v>
+        <v>155</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>190</v>
+        <v>156</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="1"/>
@@ -2428,13 +2428,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>192</v>
+        <v>157</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="1"/>
@@ -2444,16 +2444,16 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>193</v>
+        <v>158</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>194</v>
+        <v>159</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>195</v>
+        <v>160</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -2462,13 +2462,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>196</v>
+        <v>161</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>197</v>
+        <v>162</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="1"/>
@@ -2478,13 +2478,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>198</v>
+        <v>163</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>199</v>
+        <v>164</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="1"/>
@@ -2494,13 +2494,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>200</v>
+        <v>165</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>201</v>
+        <v>166</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="1"/>
@@ -2510,16 +2510,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>202</v>
+        <v>167</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -2528,34 +2528,34 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>204</v>
+        <v>168</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>205</v>
+        <v>169</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>189</v>
+        <v>155</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>206</v>
+        <v>170</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="1"/>
@@ -2565,16 +2565,16 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>205</v>
+        <v>169</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>207</v>
+        <v>171</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -2583,13 +2583,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>209</v>
+        <v>172</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>189</v>
+        <v>155</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>210</v>
+        <v>173</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="1"/>
@@ -2599,27 +2599,27 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>209</v>
+        <v>172</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>211</v>
+        <v>174</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>212</v>
+        <v>228</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -2627,16 +2627,16 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
@@ -2644,16 +2644,16 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -2661,16 +2661,16 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -2678,13 +2678,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
@@ -2693,16 +2693,16 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>101</v>
+        <v>207</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -2710,16 +2710,16 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>100</v>
+        <v>208</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
@@ -2727,36 +2727,36 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>224</v>
+        <v>181</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
       <c r="F23" s="7" t="s">
-        <v>225</v>
+        <v>182</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H23" t="s">
-        <v>226</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
@@ -2764,16 +2764,16 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
@@ -2781,16 +2781,16 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
@@ -2798,16 +2798,16 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
@@ -2815,13 +2815,13 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
@@ -2830,16 +2830,16 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
@@ -2847,376 +2847,376 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>224</v>
+        <v>181</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7" t="s">
-        <v>225</v>
+        <v>182</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H31" t="s">
-        <v>226</v>
+        <v>183</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D32" s="7"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>224</v>
+        <v>181</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7" t="s">
-        <v>225</v>
+        <v>182</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H35" t="s">
-        <v>226</v>
+        <v>183</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="D36" s="7"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
-        <v>229</v>
+        <v>186</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>224</v>
+        <v>181</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
       <c r="F39" s="7" t="s">
-        <v>225</v>
+        <v>182</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H39" t="s">
-        <v>226</v>
+        <v>183</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D40" s="7"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>224</v>
+        <v>181</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7" t="s">
-        <v>225</v>
+        <v>182</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H43" t="s">
-        <v>226</v>
+        <v>183</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="D44" s="7"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>224</v>
+        <v>181</v>
       </c>
       <c r="C47" s="8"/>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
       <c r="F47" s="7" t="s">
-        <v>225</v>
+        <v>182</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H47" t="s">
-        <v>226</v>
+        <v>183</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="D48" s="7"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>224</v>
+        <v>181</v>
       </c>
       <c r="C51" s="8"/>
       <c r="D51" s="7"/>
       <c r="E51" s="7"/>
       <c r="F51" s="7" t="s">
-        <v>225</v>
+        <v>182</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H51" t="s">
-        <v>226</v>
+        <v>183</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
-        <v>164</v>
+        <v>134</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>165</v>
+        <v>135</v>
       </c>
       <c r="D52" s="7"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
-        <v>164</v>
+        <v>134</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>166</v>
+        <v>136</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
-        <v>164</v>
+        <v>134</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>167</v>
+        <v>137</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>168</v>
+        <v>138</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F54" s="9"/>
       <c r="G54" s="7"/>
@@ -3224,671 +3224,671 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
-        <v>164</v>
+        <v>134</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>224</v>
+        <v>181</v>
       </c>
       <c r="C55" s="8"/>
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
       <c r="F55" s="7" t="s">
-        <v>225</v>
+        <v>182</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H55" t="s">
-        <v>226</v>
+        <v>183</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>173</v>
+        <v>142</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>76</v>
+        <v>206</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>77</v>
+        <v>209</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>86</v>
+        <v>210</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>87</v>
+        <v>211</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>78</v>
+        <v>212</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>89</v>
+        <v>213</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>97</v>
+        <v>214</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>169</v>
+        <v>215</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>113</v>
+        <v>221</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>111</v>
+        <v>216</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>174</v>
+        <v>195</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>115</v>
+        <v>218</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>116</v>
+        <v>219</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>117</v>
+        <v>220</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>139</v>
+        <v>196</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>140</v>
+        <v>197</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>175</v>
+        <v>225</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>176</v>
+        <v>226</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="D75" s="7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="D77" s="7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="7" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="D78" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>179</v>
+        <v>145</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="7" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="D80" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="7" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="7" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="D82" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="7" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="D83" s="7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="D84" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="D85" s="7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="D86" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>145</v>
+        <v>198</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>146</v>
+        <v>121</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>147</v>
+        <v>199</v>
       </c>
       <c r="D88" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="7" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>148</v>
+        <v>122</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>152</v>
+        <v>200</v>
       </c>
       <c r="D89" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="7" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>153</v>
+        <v>224</v>
       </c>
       <c r="D90" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="7" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>154</v>
+        <v>222</v>
       </c>
       <c r="D91" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="7" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>149</v>
+        <v>123</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>155</v>
+        <v>223</v>
       </c>
       <c r="D92" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="7" t="s">
-        <v>156</v>
+        <v>126</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="D93" s="7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="7" t="s">
-        <v>156</v>
+        <v>126</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="D94" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
-        <v>157</v>
+        <v>127</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>161</v>
+        <v>131</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
-        <v>157</v>
+        <v>127</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
       <c r="D96" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="7" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>170</v>
+        <v>139</v>
       </c>
       <c r="D97" s="7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="7" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>184</v>
+        <v>150</v>
       </c>
       <c r="D98" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="7" t="s">
-        <v>225</v>
+        <v>182</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>226</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C57" r:id="rId1" xr:uid="{33CD0375-FDC4-864D-8BAE-CF58136577F6}"/>
-    <hyperlink ref="C58" r:id="rId2" xr:uid="{87955B5B-4B6D-4B4A-B115-3F447052E311}"/>
-    <hyperlink ref="C61" r:id="rId3" xr:uid="{3D40A9A3-79A8-4048-A619-0101D21BBBDB}"/>
-    <hyperlink ref="C59" r:id="rId4" xr:uid="{DF6AE900-F5E5-1A46-90FE-9B17C12CD5EA}"/>
-    <hyperlink ref="C60" r:id="rId5" xr:uid="{26286F07-CF01-3D4F-AF7E-24B1DFF4CAC5}"/>
-    <hyperlink ref="C62" r:id="rId6" xr:uid="{250FC759-8E91-AD4E-BB93-AAF3872DC404}"/>
-    <hyperlink ref="C64" r:id="rId7" xr:uid="{5D2E891D-0452-324E-AC63-3B5EB8FCC576}"/>
-    <hyperlink ref="C21" r:id="rId8" xr:uid="{B83A9430-8469-3340-8A32-6DDD9D53D7BD}"/>
-    <hyperlink ref="C22" r:id="rId9" xr:uid="{699A6F69-F379-0348-B5C9-C25D7DB140FB}"/>
-    <hyperlink ref="C65" r:id="rId10" xr:uid="{EFCC2B08-8773-C547-9417-6D50A357579D}"/>
-    <hyperlink ref="C66" r:id="rId11" xr:uid="{4ED7AA7D-0161-9048-913F-4E262F489078}"/>
-    <hyperlink ref="C68" r:id="rId12" xr:uid="{D4B94815-2A3D-554A-9A3A-D6C41768932F}"/>
-    <hyperlink ref="C69" r:id="rId13" xr:uid="{B9A4BC97-C4E7-CB40-BDEE-3FC54B1A15F8}"/>
-    <hyperlink ref="C70" r:id="rId14" xr:uid="{1A254817-AA29-4349-9F3D-1F08E4B7BC6D}"/>
-    <hyperlink ref="C71" r:id="rId15" location="{Reaction_medium}Medium" xr:uid="{9FFFB41F-40DA-E844-8105-33FA71783875}"/>
-    <hyperlink ref="C72" r:id="rId16" location="{Operation_mode}Mode" xr:uid="{E49C1ABB-2410-D945-BAD5-E813751ECA22}"/>
-    <hyperlink ref="C87" r:id="rId17" location="{Light_source}LightSource" xr:uid="{5D5BAA03-A593-D246-AA1D-DD5A58EEB0FF}"/>
-    <hyperlink ref="C88" r:id="rId18" location="{Lamp}Lamp" xr:uid="{B474DE65-6CF2-6449-8CB9-C1A8F1227029}"/>
-    <hyperlink ref="C89" r:id="rId19" location="{Wavelength_nm}WL" xr:uid="{CDAAFAD0-E55A-C64F-A0E5-874107AAA07C}"/>
-    <hyperlink ref="C90" r:id="rId20" xr:uid="{D635B011-750E-414E-91E7-5327241CF37A}"/>
+    <hyperlink ref="C57" r:id="rId1" display="http://w3id.org/solar/i/Input/Catalyst/{ID}-{Catalyst}" xr:uid="{33CD0375-FDC4-864D-8BAE-CF58136577F6}"/>
+    <hyperlink ref="C58" r:id="rId2" display="http://w3id.org/solar/i/Input/Co-catalyst/{ID}-{Co_catalyst}" xr:uid="{87955B5B-4B6D-4B4A-B115-3F447052E311}"/>
+    <hyperlink ref="C61" r:id="rId3" display="http://w3id.org/solar/i/Input/Support/{ID}-{Support}" xr:uid="{3D40A9A3-79A8-4048-A619-0101D21BBBDB}"/>
+    <hyperlink ref="C59" r:id="rId4" display="http://w3id.org/solar/i/Input/Co-catalyst/{ID}-{co_catalyst_2}" xr:uid="{DF6AE900-F5E5-1A46-90FE-9B17C12CD5EA}"/>
+    <hyperlink ref="C60" r:id="rId5" display="http://w3id.org/solar/i/Input/Co-catalyst/{ID}-{co_catalyst_3}" xr:uid="{26286F07-CF01-3D4F-AF7E-24B1DFF4CAC5}"/>
+    <hyperlink ref="C62" r:id="rId6" display="http://w3id.org/solar/i/Input/Dopant/{ID}-{Dopant}" xr:uid="{250FC759-8E91-AD4E-BB93-AAF3872DC404}"/>
+    <hyperlink ref="C64" r:id="rId7" display="http://w3id.org/solar/i/Input/Reductant/{ID}-{Reductant}" xr:uid="{5D2E891D-0452-324E-AC63-3B5EB8FCC576}"/>
+    <hyperlink ref="C21" r:id="rId8" display="http://w3id.org/solar/i/BandGap/{ID}-{Catalyst}" xr:uid="{B83A9430-8469-3340-8A32-6DDD9D53D7BD}"/>
+    <hyperlink ref="C22" r:id="rId9" display="http://w3id.org/solar/i/SurfaceArea/{ID}-{Catalyst}" xr:uid="{699A6F69-F379-0348-B5C9-C25D7DB140FB}"/>
+    <hyperlink ref="C65" r:id="rId10" display="http://w3id.org/solar/i/Condition/LightSource/{ID}" xr:uid="{EFCC2B08-8773-C547-9417-6D50A357579D}"/>
+    <hyperlink ref="C66" r:id="rId11" display="http://w3id.org/solar/i/Condition/pH/{ID}" xr:uid="{4ED7AA7D-0161-9048-913F-4E262F489078}"/>
+    <hyperlink ref="C68" r:id="rId12" display="http://w3id.org/solar/i/Condition/Pressure/{ID}" xr:uid="{D4B94815-2A3D-554A-9A3A-D6C41768932F}"/>
+    <hyperlink ref="C69" r:id="rId13" display="http://w3id.org/solar/i/Condition/Temperature/{ID}" xr:uid="{B9A4BC97-C4E7-CB40-BDEE-3FC54B1A15F8}"/>
+    <hyperlink ref="C70" r:id="rId14" display="http://w3id.org/solar/i/Condition/Time/{ID}" xr:uid="{1A254817-AA29-4349-9F3D-1F08E4B7BC6D}"/>
+    <hyperlink ref="C71" r:id="rId15" location="{Reaction_medium}Medium" display="http://w3id.org/solar/o/core#{Reaction_medium}Medium" xr:uid="{9FFFB41F-40DA-E844-8105-33FA71783875}"/>
+    <hyperlink ref="C72" r:id="rId16" location="{Operation_mode}Mode" display="http://w3id.org/solar/o/core#{Operation_mode}Mode" xr:uid="{E49C1ABB-2410-D945-BAD5-E813751ECA22}"/>
+    <hyperlink ref="C87" r:id="rId17" location="{Light_source}LightSource" display="http://w3id.org/solar/o/core#{Light_source}LightSource" xr:uid="{5D5BAA03-A593-D246-AA1D-DD5A58EEB0FF}"/>
+    <hyperlink ref="C88" r:id="rId18" location="{Lamp}Lamp" display="http://w3id.org/solar/o/core#{Lamp}Lamp" xr:uid="{B474DE65-6CF2-6449-8CB9-C1A8F1227029}"/>
+    <hyperlink ref="C89" r:id="rId19" location="{Wavelength_nm}WL" display="http://w3id.org/solar/o/core#{Wavelength_nm}WL" xr:uid="{CDAAFAD0-E55A-C64F-A0E5-874107AAA07C}"/>
+    <hyperlink ref="C90" r:id="rId20" display="http://w3id.org/solar/i/IlluminatedArea/{ID}" xr:uid="{D635B011-750E-414E-91E7-5327241CF37A}"/>
     <hyperlink ref="C91:C92" r:id="rId21" display="http://w3id.org/solar/i/IlluminatedArea/{ID}" xr:uid="{4DFEDC35-DAA6-804C-B0F6-2CAF9BC91727}"/>
-    <hyperlink ref="C91" r:id="rId22" xr:uid="{1D48B95E-8BAD-E044-A7A5-74EFE823C221}"/>
-    <hyperlink ref="C92" r:id="rId23" xr:uid="{6118BC49-CEA9-7C4E-ABE8-63EA5ED604C9}"/>
-    <hyperlink ref="C63" r:id="rId24" xr:uid="{BD436ABE-9765-184F-AB49-2AAD056EA2AC}"/>
-    <hyperlink ref="C67" r:id="rId25" location="{Reactor_type}Reactor" xr:uid="{12796564-401A-904D-BA88-6DE0252945FE}"/>
-    <hyperlink ref="C74" r:id="rId26" xr:uid="{4A57F8C9-3F6B-F346-9C06-14ACCD76C291}"/>
-    <hyperlink ref="C73" r:id="rId27" xr:uid="{D05AEF8F-000B-5243-AA02-25149BFE83E8}"/>
-    <hyperlink ref="C15" r:id="rId28" xr:uid="{2503A0AF-6306-B442-BAF4-FE5558F49054}"/>
-    <hyperlink ref="C13" r:id="rId29" xr:uid="{43608D61-A942-0444-9531-A10AB9261A99}"/>
-    <hyperlink ref="C10" r:id="rId30" xr:uid="{4A64E9B0-01B7-7B4D-9DDC-33AFEBA4C9E6}"/>
-    <hyperlink ref="C56" r:id="rId31" xr:uid="{590C6980-47B5-A946-AD9A-4A310BA4F056}"/>
+    <hyperlink ref="C91" r:id="rId22" display="http://w3id.org/solar/i/Power/{ID}" xr:uid="{1D48B95E-8BAD-E044-A7A5-74EFE823C221}"/>
+    <hyperlink ref="C92" r:id="rId23" display="http://w3id.org/solar/i/Irradiance/{ID}" xr:uid="{6118BC49-CEA9-7C4E-ABE8-63EA5ED604C9}"/>
+    <hyperlink ref="C63" r:id="rId24" display="http://w3id.org/solar/i/Input/Dye/{ID}-{Dyes}" xr:uid="{BD436ABE-9765-184F-AB49-2AAD056EA2AC}"/>
+    <hyperlink ref="C67" r:id="rId25" location="{Reactor_type}Reactor" display="http://w3id.org/solar/o/core#{Reactor_type}Reactor" xr:uid="{12796564-401A-904D-BA88-6DE0252945FE}"/>
+    <hyperlink ref="C74" r:id="rId26" display="http://w3id.org/solar/i/Condition/ReactorResidenceTime/{ID}" xr:uid="{4A57F8C9-3F6B-F346-9C06-14ACCD76C291}"/>
+    <hyperlink ref="C73" r:id="rId27" display="http://w3id.org/solar/i/Condition/ReactorVolume/{ID}" xr:uid="{D05AEF8F-000B-5243-AA02-25149BFE83E8}"/>
+    <hyperlink ref="C15" r:id="rId28" display="http://w3id.org/solar/i/Country/{institutions.country_code}" xr:uid="{2503A0AF-6306-B442-BAF4-FE5558F49054}"/>
+    <hyperlink ref="C13" r:id="rId29" display="http://w3id.org/solar/i/Affiliation/{institutions.id}" xr:uid="{43608D61-A942-0444-9531-A10AB9261A99}"/>
+    <hyperlink ref="C10" r:id="rId30" display="http://w3id.org/solar/i/Author/{authorships.author.orcid}" xr:uid="{4A64E9B0-01B7-7B4D-9DDC-33AFEBA4C9E6}"/>
+    <hyperlink ref="C56" r:id="rId31" display="http://w3id.org/solar/i/Article/{No_de_Ref}" xr:uid="{590C6980-47B5-A946-AD9A-4A310BA4F056}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>